<commit_message>
LSP added to development
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksnelling/Desktop/form-creator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD4551D2-6B74-6143-BE55-F670EB7139B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F6DF2C-B125-0746-8D3B-08BCC97057FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="880" windowWidth="19900" windowHeight="20560" xr2:uid="{5B803FEE-CBC5-CD4B-BFE8-7DF0DABD6B40}"/>
+    <workbookView xWindow="18000" yWindow="880" windowWidth="18000" windowHeight="20500" xr2:uid="{5B803FEE-CBC5-CD4B-BFE8-7DF0DABD6B40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="127">
   <si>
     <t>patient_name</t>
   </si>
@@ -363,6 +363,60 @@
   </si>
   <si>
     <t>Emotional support</t>
+  </si>
+  <si>
+    <t>LSP</t>
+  </si>
+  <si>
+    <t>LSP Values</t>
+  </si>
+  <si>
+    <t>Difficulty initiaiting and responding to conversation?</t>
+  </si>
+  <si>
+    <t>Does this person generally withdraw from social contact?</t>
+  </si>
+  <si>
+    <t>Does this person generally show warmth to others?</t>
+  </si>
+  <si>
+    <t>Is this person generally well groomed?</t>
+  </si>
+  <si>
+    <t>Does this person wear clean clothes generally?</t>
+  </si>
+  <si>
+    <t>Does this person generally neglect her or his physical health?</t>
+  </si>
+  <si>
+    <t>Is this person violent to others?</t>
+  </si>
+  <si>
+    <t>Does this person generally make and/or keep friendships?</t>
+  </si>
+  <si>
+    <t>Does this personal generally look after their own medication?</t>
+  </si>
+  <si>
+    <t>Is this person willing to take psychiatric medication when prescribed?</t>
+  </si>
+  <si>
+    <t>Does this person generally maintain an adequate diet?</t>
+  </si>
+  <si>
+    <t>Does this person cooperate with health services?</t>
+  </si>
+  <si>
+    <t>Does this person generally have problems living with others?</t>
+  </si>
+  <si>
+    <t>Does this person behave offensively?</t>
+  </si>
+  <si>
+    <t>Does this person behave irresponsibly?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What sort of work is this person capable of? </t>
   </si>
 </sst>
 </file>
@@ -398,7 +452,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -423,6 +477,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -439,9 +499,6 @@
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -477,6 +534,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45B32DC-4C24-CA4A-AFD2-C2BFFA6D046C}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -834,649 +892,736 @@
     <col min="7" max="7" width="39.5" customWidth="1"/>
     <col min="8" max="8" width="19.1640625" customWidth="1"/>
     <col min="9" max="9" width="19.6640625" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="59.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="I1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="6">
+      <c r="E2" s="8"/>
+      <c r="F2" s="5">
         <v>1</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="5" t="s">
+      <c r="J2" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K2" s="12"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="6">
+      <c r="E3" s="8"/>
+      <c r="F3" s="5">
         <v>2</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="5" t="s">
+      <c r="J3" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="K3" s="12"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="6">
+      <c r="E4" s="8"/>
+      <c r="F4" s="5">
         <v>3</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="5" t="s">
+      <c r="J4" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="K4" s="12"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="6">
+      <c r="E5" s="8"/>
+      <c r="F5" s="5">
         <v>4</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="H5" s="6"/>
+      <c r="I5" s="5">
+        <v>4</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="K5" s="12"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="6">
+      <c r="E6" s="8"/>
+      <c r="F6" s="5">
         <v>5</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H6" s="6"/>
+      <c r="I6" s="5">
+        <v>5</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="K6" s="12"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="6">
+      <c r="E7" s="8"/>
+      <c r="F7" s="5">
         <v>6</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H7" s="6"/>
+      <c r="I7" s="5">
+        <v>6</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="K7" s="12"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="6">
+      <c r="E8" s="8"/>
+      <c r="F8" s="5">
         <v>7</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H8" s="6"/>
+      <c r="I8" s="5">
+        <v>7</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="K8" s="12"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="6">
+      <c r="E9" s="8"/>
+      <c r="F9" s="5">
         <v>8</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H9" s="6"/>
+      <c r="I9" s="5">
+        <v>8</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="6">
+      <c r="E10" s="8"/>
+      <c r="F10" s="5">
         <v>9</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H10" s="6"/>
+      <c r="I10" s="5">
+        <v>9</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="6">
+      <c r="E11" s="8"/>
+      <c r="F11" s="5">
         <v>10</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H11" s="6"/>
+      <c r="I11" s="5">
+        <v>10</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="K11" s="12"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="6">
+      <c r="E12" s="8"/>
+      <c r="F12" s="5">
         <v>11</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H12" s="6"/>
+      <c r="I12" s="5">
+        <v>11</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="K12" s="12"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="6">
+      <c r="E13" s="8"/>
+      <c r="F13" s="5">
         <v>12</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H13" s="6"/>
+      <c r="I13" s="5">
+        <v>12</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="K13" s="12"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="6">
+      <c r="E14" s="8"/>
+      <c r="F14" s="5">
         <v>13</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="H14" s="7"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H14" s="6"/>
+      <c r="I14" s="5">
+        <v>13</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="K14" s="12"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="6">
+      <c r="E15" s="8"/>
+      <c r="F15" s="5">
         <v>14</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H15" s="6"/>
+      <c r="I15" s="5">
+        <v>14</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="K15" s="12"/>
+    </row>
+    <row r="16" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="6">
+      <c r="E16" s="8"/>
+      <c r="F16" s="5">
         <v>15</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H16" s="9"/>
+      <c r="I16" s="5">
+        <v>15</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="6">
+      <c r="E17" s="8"/>
+      <c r="F17" s="5">
         <v>16</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G17" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H17" s="10"/>
+      <c r="I17" s="5">
+        <v>16</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="6">
+      <c r="E18" s="8"/>
+      <c r="F18" s="5">
         <v>17</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="H18" s="11"/>
+      <c r="H18" s="10"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="6">
+      <c r="E19" s="8"/>
+      <c r="F19" s="5">
         <v>18</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="H19" s="11"/>
+      <c r="H19" s="10"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="6">
+      <c r="E20" s="8"/>
+      <c r="F20" s="5">
         <v>19</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="H20" s="11"/>
+      <c r="H20" s="10"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="6">
+      <c r="E21" s="8"/>
+      <c r="F21" s="5">
         <v>20</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="H21" s="11"/>
+      <c r="H21" s="10"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="6">
+      <c r="E22" s="8"/>
+      <c r="F22" s="5">
         <v>21</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="G22" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="H22" s="7"/>
+      <c r="H22" s="6"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="6">
+      <c r="E23" s="8"/>
+      <c r="F23" s="5">
         <v>22</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="H23" s="10"/>
+      <c r="H23" s="9"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="9"/>
-      <c r="F24" s="6">
+      <c r="E24" s="8"/>
+      <c r="F24" s="5">
         <v>23</v>
       </c>
-      <c r="G24" s="12" t="s">
+      <c r="G24" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="H24" s="11"/>
+      <c r="H24" s="10"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="6">
+      <c r="E25" s="8"/>
+      <c r="F25" s="5">
         <v>24</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G25" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="H25" s="11"/>
+      <c r="H25" s="10"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="6">
+      <c r="E26" s="8"/>
+      <c r="F26" s="5">
         <v>25</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="G26" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="H26" s="11"/>
+      <c r="H26" s="10"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="6">
+      <c r="E27" s="8"/>
+      <c r="F27" s="5">
         <v>26</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G27" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="H27" s="11"/>
+      <c r="H27" s="10"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="6">
+      <c r="E28" s="8"/>
+      <c r="F28" s="5">
         <v>27</v>
       </c>
-      <c r="G28" s="12" t="s">
+      <c r="G28" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="H28" s="11"/>
+      <c r="H28" s="10"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="6">
+      <c r="E29" s="8"/>
+      <c r="F29" s="5">
         <v>28</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="G29" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="H29" s="7"/>
+      <c r="H29" s="6"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E30" s="9"/>
+      <c r="E30" s="8"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E31" s="9"/>
+      <c r="E31" s="8"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="9"/>
+      <c r="E32" s="8"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -1486,13 +1631,13 @@
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E33" s="9"/>
+      <c r="E33" s="8"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -1502,13 +1647,13 @@
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E34" s="9"/>
+      <c r="E34" s="8"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -1518,13 +1663,13 @@
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E35" s="9"/>
+      <c r="E35" s="8"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -1534,13 +1679,13 @@
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="E36" s="9"/>
+      <c r="E36" s="8"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -1548,16 +1693,16 @@
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="E37" s="9"/>
+      <c r="E37" s="8"/>
     </row>
   </sheetData>
-  <dataValidations count="7">
+  <dataValidations count="8">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Enter an integer between 0 and 120" sqref="B3" xr:uid="{B1ED41BC-30F7-C54A-AE94-8016912BA55A}">
       <formula1>0</formula1>
       <formula2>120</formula2>
@@ -1582,6 +1727,10 @@
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" sqref="K2:K17" xr:uid="{F40569F7-7A99-BB41-9B25-EBAC446CE1DB}">
+      <formula1>0</formula1>
+      <formula2>3</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
minor bugs rectified with case-sensitivity with Lawton and Berg missing option 4
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksnelling/Desktop/form-creator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB01A9C2-BD2E-3849-AD35-8E74537D951A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7A9C12-903A-3F44-8BCE-4362796D78E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18020" yWindow="880" windowWidth="17980" windowHeight="20500" xr2:uid="{5B803FEE-CBC5-CD4B-BFE8-7DF0DABD6B40}"/>
   </bookViews>
@@ -1324,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45B32DC-4C24-CA4A-AFD2-C2BFFA6D046C}">
   <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3108,7 +3108,7 @@
       <c r="Z37" s="15"/>
     </row>
   </sheetData>
-  <dataValidations count="19">
+  <dataValidations count="20">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Enter an integer between 0 and 120" sqref="B4" xr:uid="{B1ED41BC-30F7-C54A-AE94-8016912BA55A}">
       <formula1>0</formula1>
       <formula2>120</formula2>
@@ -3140,7 +3140,7 @@
       <formula1>1</formula1>
       <formula2>3</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input an integer between 0 and 4" sqref="Q2:Q15 T2:T21" xr:uid="{CEC098AE-182D-FA49-8CF0-EEB9E0847019}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input an integer between 0 and 4" sqref="Q2:Q15" xr:uid="{CEC098AE-182D-FA49-8CF0-EEB9E0847019}">
       <formula1>0</formula1>
       <formula2>4</formula2>
     </dataValidation>
@@ -3175,6 +3175,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input either 'Y' or 'N'" sqref="Z10:Z19" xr:uid="{C45CB5A2-312A-9349-BC4A-AA78049DC6D5}">
       <formula1>"Y, N"</formula1>
     </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input an integer between 0 and 4" sqref="T2:T21" xr:uid="{2D8109B5-D74A-8546-B0A9-B4F4B20ADC41}">
+      <formula1>0</formula1>
+      <formula2>3</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
altered data validation for LEFS
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksnelling/Desktop/form-creator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7A9C12-903A-3F44-8BCE-4362796D78E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34EDADD-E16B-4740-BAE1-20F760EC560C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18020" yWindow="880" windowWidth="17980" windowHeight="20500" xr2:uid="{5B803FEE-CBC5-CD4B-BFE8-7DF0DABD6B40}"/>
   </bookViews>
@@ -1324,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45B32DC-4C24-CA4A-AFD2-C2BFFA6D046C}">
   <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3175,9 +3175,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input either 'Y' or 'N'" sqref="Z10:Z19" xr:uid="{C45CB5A2-312A-9349-BC4A-AA78049DC6D5}">
       <formula1>"Y, N"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input an integer between 0 and 4" sqref="T2:T21" xr:uid="{2D8109B5-D74A-8546-B0A9-B4F4B20ADC41}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input a number between 0 and 4" sqref="T2:T21" xr:uid="{A7F9FF7C-FF09-EC46-BFD7-DDA6C142E68D}">
       <formula1>0</formula1>
-      <formula2>3</formula2>
+      <formula2>4</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
basic error handling included with alert messages.
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksnelling/Desktop/form-creator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34EDADD-E16B-4740-BAE1-20F760EC560C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1095B92-7E7D-2E41-B178-82B9ACED03E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18020" yWindow="880" windowWidth="17980" windowHeight="20500" xr2:uid="{5B803FEE-CBC5-CD4B-BFE8-7DF0DABD6B40}"/>
+    <workbookView xWindow="18040" yWindow="880" windowWidth="17960" windowHeight="20420" xr2:uid="{5B803FEE-CBC5-CD4B-BFE8-7DF0DABD6B40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="280">
   <si>
     <t>age</t>
   </si>
@@ -429,27 +429,6 @@
   </si>
   <si>
     <t>H</t>
-  </si>
-  <si>
-    <t>Ability to Use Telephone</t>
-  </si>
-  <si>
-    <t>Food Preparation</t>
-  </si>
-  <si>
-    <t>Housekeeping</t>
-  </si>
-  <si>
-    <t>Laundry</t>
-  </si>
-  <si>
-    <t>Mode of Transportation</t>
-  </si>
-  <si>
-    <t>Reponsibility for Own Medications</t>
-  </si>
-  <si>
-    <t>Ability to Handle Finances</t>
   </si>
   <si>
     <t>ndis_no</t>
@@ -832,11 +811,217 @@
       <t>(specify below)</t>
     </r>
   </si>
+  <si>
+    <t>Concentrating for 10 minutes at a time</t>
+  </si>
+  <si>
+    <t>Remembering to do important things</t>
+  </si>
+  <si>
+    <t>Finding a way to deal with every day common problems</t>
+  </si>
+  <si>
+    <t>Learning how to do something new</t>
+  </si>
+  <si>
+    <t>Generally understanding what people say</t>
+  </si>
+  <si>
+    <t>Telling your family or firneds about things</t>
+  </si>
+  <si>
+    <t>Standing for a reasonable period of time</t>
+  </si>
+  <si>
+    <t>Getting up from a sitting position</t>
+  </si>
+  <si>
+    <t>Moving around inside uyour home</t>
+  </si>
+  <si>
+    <t>Getting around at school or at a friend's</t>
+  </si>
+  <si>
+    <t>Walking for as long a distance as other people your age</t>
+  </si>
+  <si>
+    <t>Keeping yourself and your clothes clean, taking baths or shower and brushing your teeth without being asked</t>
+  </si>
+  <si>
+    <t>Getting dressed on your own</t>
+  </si>
+  <si>
+    <t>Eating meals without help</t>
+  </si>
+  <si>
+    <t>Staying safe when you are alone or not putting 
+yourself in danger when there are no adults around</t>
+  </si>
+  <si>
+    <t>Getting along with people you do not know well</t>
+  </si>
+  <si>
+    <t>Keeping a friendship</t>
+  </si>
+  <si>
+    <t>Getting along with family members</t>
+  </si>
+  <si>
+    <t>Getting along with teachers or adults not in your family</t>
+  </si>
+  <si>
+    <t>Doing chores or other things you are expected to do at home</t>
+  </si>
+  <si>
+    <t>Finishing chores or home activities that you are supposed to do</t>
+  </si>
+  <si>
+    <t>Doing chores or other home activities well</t>
+  </si>
+  <si>
+    <t>Doing home activities quickly when it is important</t>
+  </si>
+  <si>
+    <t>Joining in on community activities</t>
+  </si>
+  <si>
+    <t>Getting invited to parties, play dates, hanging out</t>
+  </si>
+  <si>
+    <t>How much time do your parents spend on your health condition</t>
+  </si>
+  <si>
+    <t>How much have you been upset by your health condition</t>
+  </si>
+  <si>
+    <t>How much of a problem do you have doing things you enjoy</t>
+  </si>
+  <si>
+    <r>
+      <t>Doing your regular school assignments</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> (if not relevant leave empty)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Following the rules or fitting in with others </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> (if not relevant leave empty)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Getting your school work done as quickly as needed  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(if not relevant leave empty)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Completing all of the school assignment that you need to do  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(if not relevant leave empty)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Studying for important school tests  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(if not relevant leave empty)</t>
+    </r>
+  </si>
+  <si>
+    <t>WHODASKIDS</t>
+  </si>
+  <si>
+    <t>WHODASKIDS Values</t>
+  </si>
+  <si>
+    <t>1. Operates telephone on own initiative
+2. Dials a few well-known numbers
+3. Answers telephone but does not dial
+4. Does not use telephone at all</t>
+  </si>
+  <si>
+    <t>1. Takes care of all shopping needs independently
+2. Shops independently for small purchases
+3. Needs to be accompanied on any shopping trip
+4. Completely unable to shop</t>
+  </si>
+  <si>
+    <t>1. Plans, prepares and serves adequate meals independently
+2. Prepares adequate meals if supplied with ingredients
+3. Heats, serves and prepares meals but does not maintain adequate diet
+4. Needs to have meals prepared and served</t>
+  </si>
+  <si>
+    <t>1. Maintains house alone or with occasional assistance
+2. Performs light daily tasks
+3. Performs light daily tasks but cannot maintain suitable cleanliness
+4. Needs help with all home maintenance
+5. Does not participate in any housekeeping</t>
+  </si>
+  <si>
+    <t>1. Does personal laundry completely
+2. Launders small items
+3. All laundry must be done by others</t>
+  </si>
+  <si>
+    <t>1. Travels independently on public transportation or drives own car
+2. Arranges own travel via taxi
+3. Travels on public transport when accompanied
+4. Travel limited to taxi or autombile with others
+5. Does not travel</t>
+  </si>
+  <si>
+    <t>1. Is responsible for taking medication in correct dosages at correct time
+2. Takes responsibility if medication is prepared in advance
+3. Is not capable of dispensing own medication</t>
+  </si>
+  <si>
+    <t>1. Manages financial matters independently, collects and keeps track of income
+2. Manages day-to-day purchases, but needs help with banking, major purchases
+3. Inncapable of handling money</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -904,7 +1089,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -927,11 +1112,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -955,10 +1153,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -980,6 +1174,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1322,10 +1538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45B32DC-4C24-CA4A-AFD2-C2BFFA6D046C}">
-  <dimension ref="A1:Z37"/>
+  <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1341,7 +1557,7 @@
     <col min="9" max="9" width="19.6640625" customWidth="1"/>
     <col min="10" max="10" width="59.1640625" customWidth="1"/>
     <col min="12" max="12" width="13.1640625" customWidth="1"/>
-    <col min="13" max="13" width="28.83203125" customWidth="1"/>
+    <col min="13" max="13" width="71.1640625" customWidth="1"/>
     <col min="14" max="14" width="18" customWidth="1"/>
     <col min="15" max="15" width="10.83203125" customWidth="1"/>
     <col min="16" max="16" width="63.1640625" customWidth="1"/>
@@ -1349,13 +1565,16 @@
     <col min="19" max="19" width="45.33203125" customWidth="1"/>
     <col min="21" max="21" width="16.83203125" customWidth="1"/>
     <col min="22" max="22" width="55.5" customWidth="1"/>
-    <col min="24" max="24" width="10.83203125" style="14"/>
-    <col min="25" max="25" width="49.33203125" style="14" customWidth="1"/>
-    <col min="26" max="26" width="18.5" style="14" customWidth="1"/>
-    <col min="27" max="16384" width="10.83203125" style="14"/>
+    <col min="24" max="24" width="10.83203125" style="13"/>
+    <col min="25" max="25" width="49.33203125" style="13" customWidth="1"/>
+    <col min="26" max="26" width="18.5" style="13" customWidth="1"/>
+    <col min="27" max="27" width="14.6640625" style="13" customWidth="1"/>
+    <col min="28" max="28" width="75.83203125" style="13" customWidth="1"/>
+    <col min="29" max="29" width="21.33203125" style="13" customWidth="1"/>
+    <col min="30" max="16384" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -1399,45 +1618,54 @@
         <v>122</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>221</v>
+      <c r="Z1" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA1" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="AB1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC1" s="17" t="s">
+        <v>271</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
@@ -1464,42 +1692,49 @@
       <c r="L2" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>131</v>
+      <c r="M2" s="6" t="s">
+        <v>272</v>
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="4">
         <v>1</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="Q2" s="5"/>
       <c r="R2" s="4">
         <v>1</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="T2" s="5"/>
       <c r="U2" s="4" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="W2" s="5"/>
       <c r="X2" s="4">
         <v>1</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="Z2" s="5"/>
+        <v>215</v>
+      </c>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="4">
+        <v>11</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC2" s="5"/>
     </row>
-    <row r="3" spans="1:26" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="2" t="s">
@@ -1526,40 +1761,47 @@
       <c r="L3" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="M3" s="4" t="s">
-        <v>91</v>
+      <c r="M3" s="6" t="s">
+        <v>273</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="4">
         <v>2</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="Q3" s="5"/>
       <c r="R3" s="4">
         <v>2</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="T3" s="5"/>
       <c r="U3" s="4" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="W3" s="5"/>
       <c r="X3" s="4">
         <v>2</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z3" s="5"/>
+        <v>216</v>
+      </c>
+      <c r="Z3" s="16"/>
+      <c r="AA3" s="4">
+        <v>12</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC3" s="5"/>
     </row>
-    <row r="4" spans="1:26" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1588,40 +1830,47 @@
       <c r="L4" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="M4" s="4" t="s">
-        <v>132</v>
+      <c r="M4" s="6" t="s">
+        <v>274</v>
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="4">
         <v>3</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="Q4" s="5"/>
       <c r="R4" s="4">
         <v>3</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="T4" s="5"/>
       <c r="U4" s="4" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="W4" s="5"/>
       <c r="X4" s="4">
         <v>3</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="Z4" s="5"/>
+        <v>217</v>
+      </c>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="4">
+        <v>13</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="AC4" s="5"/>
     </row>
-    <row r="5" spans="1:26" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1650,44 +1899,51 @@
       <c r="L5" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>133</v>
+      <c r="M5" s="6" t="s">
+        <v>275</v>
       </c>
       <c r="N5" s="5"/>
       <c r="O5" s="4">
         <v>4</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="Q5" s="5"/>
       <c r="R5" s="4">
         <v>4</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="T5" s="5"/>
       <c r="U5" s="4" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="V5" s="6" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="W5" s="5"/>
       <c r="X5" s="4">
         <v>4</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="Z5" s="5"/>
+        <v>218</v>
+      </c>
+      <c r="Z5" s="16"/>
+      <c r="AA5" s="4">
+        <v>14</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="AC5" s="5"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1712,40 +1968,47 @@
       <c r="L6" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="M6" s="4" t="s">
-        <v>134</v>
+      <c r="M6" s="6" t="s">
+        <v>276</v>
       </c>
       <c r="N6" s="5"/>
       <c r="O6" s="4">
         <v>5</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="Q6" s="5"/>
       <c r="R6" s="4">
         <v>5</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="T6" s="5"/>
       <c r="U6" s="4" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="W6" s="5"/>
       <c r="X6" s="4">
         <v>5</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="Z6" s="5"/>
+        <v>219</v>
+      </c>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="4">
+        <v>15</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="AC6" s="5"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>44</v>
       </c>
@@ -1774,42 +2037,49 @@
       <c r="L7" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="M7" s="4" t="s">
-        <v>135</v>
+      <c r="M7" s="6" t="s">
+        <v>277</v>
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="4">
         <v>6</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="Q7" s="5"/>
       <c r="R7" s="4">
         <v>6</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="T7" s="5"/>
       <c r="U7" s="4" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="V7" s="4" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="W7" s="5"/>
       <c r="X7" s="4">
         <v>6</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="Z7" s="5"/>
+        <v>220</v>
+      </c>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="4">
+        <v>16</v>
+      </c>
+      <c r="AB7" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="AC7" s="5"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="2" t="s">
@@ -1836,44 +2106,51 @@
       <c r="L8" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="M8" s="4" t="s">
-        <v>136</v>
+      <c r="M8" s="6" t="s">
+        <v>278</v>
       </c>
       <c r="N8" s="5"/>
       <c r="O8" s="4">
         <v>7</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="Q8" s="5"/>
       <c r="R8" s="4">
         <v>7</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="T8" s="5"/>
       <c r="U8" s="4" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="V8" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="W8" s="5"/>
       <c r="X8" s="4">
         <v>7</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="Z8" s="5"/>
+        <v>221</v>
+      </c>
+      <c r="Z8" s="16"/>
+      <c r="AA8" s="4">
+        <v>21</v>
+      </c>
+      <c r="AB8" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="AC8" s="5"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B9" s="5"/>
+        <v>148</v>
+      </c>
+      <c r="B9" s="21"/>
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1898,42 +2175,49 @@
       <c r="L9" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="M9" s="4" t="s">
-        <v>137</v>
+      <c r="M9" s="6" t="s">
+        <v>279</v>
       </c>
       <c r="N9" s="5"/>
       <c r="O9" s="4">
         <v>8</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="Q9" s="5"/>
       <c r="R9" s="4">
         <v>8</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="T9" s="5"/>
       <c r="U9" s="4" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="W9" s="5"/>
       <c r="X9" s="4">
         <v>8</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="Z9" s="5"/>
+        <v>236</v>
+      </c>
+      <c r="Z9" s="16"/>
+      <c r="AA9" s="4">
+        <v>22</v>
+      </c>
+      <c r="AB9" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="AC9" s="5"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1955,41 +2239,48 @@
         <v>115</v>
       </c>
       <c r="K10" s="5"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
       <c r="O10" s="4">
         <v>9</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="Q10" s="5"/>
       <c r="R10" s="4">
         <v>9</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="T10" s="5"/>
       <c r="U10" s="4" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="V10" s="4" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="W10" s="5"/>
       <c r="X10" s="4" t="s">
         <v>123</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="Z10" s="5"/>
+        <v>226</v>
+      </c>
+      <c r="Z10" s="16"/>
+      <c r="AA10" s="4">
+        <v>23</v>
+      </c>
+      <c r="AB10" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="AC10" s="5"/>
     </row>
-    <row r="11" spans="1:26" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
+    <row r="11" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
@@ -2011,41 +2302,48 @@
         <v>113</v>
       </c>
       <c r="K11" s="5"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
       <c r="O11" s="4">
         <v>10</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="Q11" s="5"/>
       <c r="R11" s="4">
         <v>10</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="T11" s="5"/>
       <c r="U11" s="4" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="V11" s="6" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="W11" s="5"/>
       <c r="X11" s="4" t="s">
         <v>124</v>
       </c>
       <c r="Y11" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="Z11" s="5"/>
+        <v>227</v>
+      </c>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="4">
+        <v>24</v>
+      </c>
+      <c r="AB11" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="AC11" s="5"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="2" t="s">
         <v>13</v>
       </c>
@@ -2067,41 +2365,48 @@
         <v>114</v>
       </c>
       <c r="K12" s="5"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
       <c r="O12" s="4">
         <v>11</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="Q12" s="5"/>
       <c r="R12" s="4">
         <v>11</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="T12" s="5"/>
       <c r="U12" s="4" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="V12" s="4" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="W12" s="5"/>
       <c r="X12" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="Z12" s="5"/>
+        <v>230</v>
+      </c>
+      <c r="Z12" s="16"/>
+      <c r="AA12" s="4">
+        <v>25</v>
+      </c>
+      <c r="AB12" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="AC12" s="5"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
+    <row r="13" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
@@ -2123,41 +2428,48 @@
         <v>116</v>
       </c>
       <c r="K13" s="5"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
       <c r="O13" s="4">
         <v>12</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="Q13" s="5"/>
       <c r="R13" s="4">
         <v>12</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="T13" s="5"/>
       <c r="U13" s="4" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="V13" s="4" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="W13" s="5"/>
       <c r="X13" s="4" t="s">
         <v>126</v>
       </c>
       <c r="Y13" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="Z13" s="5"/>
+        <v>231</v>
+      </c>
+      <c r="Z13" s="16"/>
+      <c r="AA13" s="4">
+        <v>31</v>
+      </c>
+      <c r="AB13" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="AC13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
@@ -2179,41 +2491,48 @@
         <v>117</v>
       </c>
       <c r="K14" s="5"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
       <c r="O14" s="4">
         <v>13</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="Q14" s="5"/>
       <c r="R14" s="4">
         <v>13</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="T14" s="5"/>
       <c r="U14" s="4" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="V14" s="4" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="W14" s="5"/>
       <c r="X14" s="4" t="s">
         <v>127</v>
       </c>
       <c r="Y14" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="Z14" s="5"/>
+        <v>232</v>
+      </c>
+      <c r="Z14" s="16"/>
+      <c r="AA14" s="4">
+        <v>32</v>
+      </c>
+      <c r="AB14" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="AC14" s="5"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
@@ -2235,41 +2554,48 @@
         <v>118</v>
       </c>
       <c r="K15" s="5"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
       <c r="O15" s="4">
         <v>14</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="Q15" s="5"/>
       <c r="R15" s="4">
         <v>14</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="T15" s="5"/>
       <c r="U15" s="4" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="V15" s="4" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="W15" s="5"/>
       <c r="X15" s="4" t="s">
         <v>128</v>
       </c>
       <c r="Y15" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="Z15" s="5"/>
+        <v>233</v>
+      </c>
+      <c r="Z15" s="16"/>
+      <c r="AA15" s="4">
+        <v>33</v>
+      </c>
+      <c r="AB15" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="AC15" s="5"/>
     </row>
-    <row r="16" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
+    <row r="16" spans="1:29" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="2" t="s">
         <v>16</v>
       </c>
@@ -2283,7 +2609,7 @@
       <c r="G16" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="H16" s="10"/>
+      <c r="H16" s="9"/>
       <c r="I16" s="4">
         <v>15</v>
       </c>
@@ -2291,24 +2617,24 @@
         <v>119</v>
       </c>
       <c r="K16" s="5"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
       <c r="R16" s="4">
         <v>15</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="T16" s="5"/>
       <c r="U16" s="4" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="V16" s="4" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="W16" s="5"/>
       <c r="X16" s="4" t="s">
@@ -2317,11 +2643,18 @@
       <c r="Y16" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="Z16" s="5"/>
+      <c r="Z16" s="16"/>
+      <c r="AA16" s="4">
+        <v>34</v>
+      </c>
+      <c r="AB16" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="AC16" s="5"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
@@ -2335,7 +2668,7 @@
       <c r="G17" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H17" s="11"/>
+      <c r="H17" s="10"/>
       <c r="I17" s="4">
         <v>16</v>
       </c>
@@ -2343,37 +2676,44 @@
         <v>120</v>
       </c>
       <c r="K17" s="5"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
       <c r="R17" s="4">
         <v>16</v>
       </c>
       <c r="S17" s="4" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="T17" s="5"/>
       <c r="U17" s="4" t="s">
         <v>84</v>
       </c>
       <c r="V17" s="4" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="W17" s="5"/>
       <c r="X17" s="4" t="s">
         <v>130</v>
       </c>
       <c r="Y17" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="Z17" s="5"/>
+        <v>234</v>
+      </c>
+      <c r="Z17" s="16"/>
+      <c r="AA17" s="4">
+        <v>41</v>
+      </c>
+      <c r="AB17" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="AC17" s="5"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="2" t="s">
         <v>19</v>
       </c>
@@ -2387,41 +2727,48 @@
       <c r="G18" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
       <c r="R18" s="4">
         <v>17</v>
       </c>
       <c r="S18" s="4" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="T18" s="5"/>
       <c r="U18" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="V18" s="13" t="s">
-        <v>213</v>
+      <c r="V18" s="12" t="s">
+        <v>206</v>
       </c>
       <c r="W18" s="5"/>
       <c r="X18" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="Y18" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="Y18" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="Z18" s="5"/>
+      <c r="Z18" s="16"/>
+      <c r="AA18" s="4">
+        <v>42</v>
+      </c>
+      <c r="AB18" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="AC18" s="5"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="2" t="s">
         <v>20</v>
       </c>
@@ -2435,41 +2782,48 @@
       <c r="G19" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
       <c r="R19" s="4">
         <v>18</v>
       </c>
       <c r="S19" s="4" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="T19" s="5"/>
       <c r="U19" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="V19" s="13" t="s">
-        <v>197</v>
+        <v>189</v>
+      </c>
+      <c r="V19" s="12" t="s">
+        <v>190</v>
       </c>
       <c r="W19" s="5"/>
       <c r="X19" s="4" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="Y19" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="Z19" s="5"/>
+      <c r="Z19" s="16"/>
+      <c r="AA19" s="4">
+        <v>43</v>
+      </c>
+      <c r="AB19" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="AC19" s="5"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="2" t="s">
         <v>21</v>
       </c>
@@ -2483,37 +2837,44 @@
       <c r="G20" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
       <c r="R20" s="4">
         <v>19</v>
       </c>
       <c r="S20" s="4" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="T20" s="5"/>
-      <c r="U20" s="12"/>
-      <c r="V20" s="12"/>
-      <c r="W20" s="12"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
       <c r="X20" s="4">
         <v>9</v>
       </c>
       <c r="Y20" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="Z20" s="5"/>
+        <v>222</v>
+      </c>
+      <c r="Z20" s="16"/>
+      <c r="AA20" s="4">
+        <v>44</v>
+      </c>
+      <c r="AB20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC20" s="5"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="2" t="s">
         <v>22</v>
       </c>
@@ -2527,37 +2888,44 @@
       <c r="G21" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H21" s="11"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
       <c r="R21" s="4">
         <v>20</v>
       </c>
       <c r="S21" s="4" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="T21" s="5"/>
-      <c r="U21" s="12"/>
-      <c r="V21" s="12"/>
-      <c r="W21" s="12"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
       <c r="X21" s="4">
         <v>10</v>
       </c>
       <c r="Y21" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="Z21" s="5"/>
+        <v>223</v>
+      </c>
+      <c r="Z21" s="16"/>
+      <c r="AA21" s="4">
+        <v>45</v>
+      </c>
+      <c r="AB21" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="AC21" s="5"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="2" t="s">
         <v>23</v>
       </c>
@@ -2572,32 +2940,39 @@
         <v>97</v>
       </c>
       <c r="H22" s="3"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="12"/>
-      <c r="V22" s="12"/>
-      <c r="W22" s="12"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
       <c r="X22" s="4">
         <v>11</v>
       </c>
       <c r="Y22" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="Z22" s="5"/>
+        <v>224</v>
+      </c>
+      <c r="Z22" s="16"/>
+      <c r="AA22" s="4">
+        <v>51</v>
+      </c>
+      <c r="AB22" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="AC22" s="5"/>
     </row>
-    <row r="23" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
+    <row r="23" spans="1:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="2" t="s">
         <v>24</v>
       </c>
@@ -2611,33 +2986,40 @@
       <c r="G23" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H23" s="10"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="12"/>
-      <c r="V23" s="12"/>
-      <c r="W23" s="12"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
       <c r="X23" s="4">
         <v>12</v>
       </c>
       <c r="Y23" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="Z23" s="5"/>
+        <v>225</v>
+      </c>
+      <c r="Z23" s="16"/>
+      <c r="AA23" s="4">
+        <v>52</v>
+      </c>
+      <c r="AB23" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="AC23" s="5"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="2" t="s">
         <v>25</v>
       </c>
@@ -2651,29 +3033,36 @@
       <c r="G24" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="H24" s="11"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
-      <c r="U24" s="12"/>
-      <c r="V24" s="12"/>
-      <c r="W24" s="12"/>
-      <c r="X24" s="15"/>
-      <c r="Y24" s="15"/>
-      <c r="Z24" s="15"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="14"/>
+      <c r="Y24" s="14"/>
+      <c r="Z24" s="14"/>
+      <c r="AA24" s="18">
+        <v>53</v>
+      </c>
+      <c r="AB24" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="AC24" s="19"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="2" t="s">
         <v>26</v>
       </c>
@@ -2687,34 +3076,41 @@
       <c r="G25" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="H25" s="11"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
-      <c r="U25" s="12"/>
-      <c r="V25" s="12"/>
-      <c r="W25" s="12"/>
-      <c r="X25" s="15"/>
-      <c r="Y25" s="15"/>
-      <c r="Z25" s="15"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="14"/>
+      <c r="Y25" s="14"/>
+      <c r="Z25" s="14"/>
+      <c r="AA25" s="18">
+        <v>54</v>
+      </c>
+      <c r="AB25" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="AC25" s="19"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="4">
@@ -2723,34 +3119,41 @@
       <c r="G26" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="H26" s="11"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
-      <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
-      <c r="U26" s="12"/>
-      <c r="V26" s="12"/>
-      <c r="W26" s="12"/>
-      <c r="X26" s="15"/>
-      <c r="Y26" s="15"/>
-      <c r="Z26" s="15"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+      <c r="X26" s="14"/>
+      <c r="Y26" s="14"/>
+      <c r="Z26" s="14"/>
+      <c r="AA26" s="18">
+        <v>55</v>
+      </c>
+      <c r="AB26" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="AC26" s="19"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="4">
@@ -2759,34 +3162,41 @@
       <c r="G27" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="H27" s="11"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
-      <c r="U27" s="12"/>
-      <c r="V27" s="12"/>
-      <c r="W27" s="12"/>
-      <c r="X27" s="15"/>
-      <c r="Y27" s="15"/>
-      <c r="Z27" s="15"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="8"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="11"/>
+      <c r="X27" s="14"/>
+      <c r="Y27" s="14"/>
+      <c r="Z27" s="14"/>
+      <c r="AA27" s="18">
+        <v>56</v>
+      </c>
+      <c r="AB27" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="AC27" s="19"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
       <c r="C28" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="4">
@@ -2795,34 +3205,41 @@
       <c r="G28" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="H28" s="11"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
-      <c r="R28" s="9"/>
-      <c r="S28" s="9"/>
-      <c r="T28" s="9"/>
-      <c r="U28" s="12"/>
-      <c r="V28" s="12"/>
-      <c r="W28" s="12"/>
-      <c r="X28" s="15"/>
-      <c r="Y28" s="15"/>
-      <c r="Z28" s="15"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
+      <c r="T28" s="8"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
+      <c r="W28" s="11"/>
+      <c r="X28" s="14"/>
+      <c r="Y28" s="14"/>
+      <c r="Z28" s="14"/>
+      <c r="AA28" s="18">
+        <v>57</v>
+      </c>
+      <c r="AB28" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="AC28" s="19"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="4">
@@ -2832,60 +3249,74 @@
         <v>87</v>
       </c>
       <c r="H29" s="3"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
-      <c r="U29" s="12"/>
-      <c r="V29" s="12"/>
-      <c r="W29" s="12"/>
-      <c r="X29" s="15"/>
-      <c r="Y29" s="15"/>
-      <c r="Z29" s="15"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="8"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+      <c r="W29" s="11"/>
+      <c r="X29" s="14"/>
+      <c r="Y29" s="14"/>
+      <c r="Z29" s="14"/>
+      <c r="AA29" s="18">
+        <v>58</v>
+      </c>
+      <c r="AB29" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="AC29" s="19"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="E30" s="3"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
-      <c r="T30" s="9"/>
-      <c r="U30" s="12"/>
-      <c r="V30" s="12"/>
-      <c r="W30" s="12"/>
-      <c r="X30" s="15"/>
-      <c r="Y30" s="15"/>
-      <c r="Z30" s="15"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="11"/>
+      <c r="W30" s="11"/>
+      <c r="X30" s="14"/>
+      <c r="Y30" s="14"/>
+      <c r="Z30" s="14"/>
+      <c r="AA30" s="18">
+        <v>59</v>
+      </c>
+      <c r="AB30" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="AC30" s="19"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="2" t="s">
         <v>32</v>
       </c>
@@ -2893,31 +3324,38 @@
         <v>71</v>
       </c>
       <c r="E31" s="3"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
-      <c r="R31" s="9"/>
-      <c r="S31" s="9"/>
-      <c r="T31" s="9"/>
-      <c r="U31" s="12"/>
-      <c r="V31" s="12"/>
-      <c r="W31" s="12"/>
-      <c r="X31" s="15"/>
-      <c r="Y31" s="15"/>
-      <c r="Z31" s="15"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="8"/>
+      <c r="T31" s="8"/>
+      <c r="U31" s="11"/>
+      <c r="V31" s="11"/>
+      <c r="W31" s="11"/>
+      <c r="X31" s="14"/>
+      <c r="Y31" s="14"/>
+      <c r="Z31" s="14"/>
+      <c r="AA31" s="18">
+        <v>61</v>
+      </c>
+      <c r="AB31" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="AC31" s="19"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
       <c r="C32" s="2" t="s">
         <v>33</v>
       </c>
@@ -2925,31 +3363,38 @@
         <v>72</v>
       </c>
       <c r="E32" s="3"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
-      <c r="R32" s="9"/>
-      <c r="S32" s="9"/>
-      <c r="T32" s="9"/>
-      <c r="U32" s="12"/>
-      <c r="V32" s="12"/>
-      <c r="W32" s="12"/>
-      <c r="X32" s="15"/>
-      <c r="Y32" s="15"/>
-      <c r="Z32" s="15"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="8"/>
+      <c r="T32" s="8"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="11"/>
+      <c r="W32" s="11"/>
+      <c r="X32" s="14"/>
+      <c r="Y32" s="14"/>
+      <c r="Z32" s="14"/>
+      <c r="AA32" s="18">
+        <v>62</v>
+      </c>
+      <c r="AB32" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC32" s="19"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="2" t="s">
         <v>34</v>
       </c>
@@ -2957,31 +3402,38 @@
         <v>73</v>
       </c>
       <c r="E33" s="3"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
-      <c r="R33" s="9"/>
-      <c r="S33" s="9"/>
-      <c r="T33" s="9"/>
-      <c r="U33" s="12"/>
-      <c r="V33" s="12"/>
-      <c r="W33" s="12"/>
-      <c r="X33" s="15"/>
-      <c r="Y33" s="15"/>
-      <c r="Z33" s="15"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="8"/>
+      <c r="U33" s="11"/>
+      <c r="V33" s="11"/>
+      <c r="W33" s="11"/>
+      <c r="X33" s="14"/>
+      <c r="Y33" s="14"/>
+      <c r="Z33" s="14"/>
+      <c r="AA33" s="18">
+        <v>63</v>
+      </c>
+      <c r="AB33" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="AC33" s="19"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="2" t="s">
         <v>35</v>
       </c>
@@ -2989,31 +3441,38 @@
         <v>74</v>
       </c>
       <c r="E34" s="3"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
-      <c r="O34" s="9"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="9"/>
-      <c r="R34" s="9"/>
-      <c r="S34" s="9"/>
-      <c r="T34" s="9"/>
-      <c r="U34" s="12"/>
-      <c r="V34" s="12"/>
-      <c r="W34" s="12"/>
-      <c r="X34" s="15"/>
-      <c r="Y34" s="15"/>
-      <c r="Z34" s="15"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="8"/>
+      <c r="U34" s="11"/>
+      <c r="V34" s="11"/>
+      <c r="W34" s="11"/>
+      <c r="X34" s="14"/>
+      <c r="Y34" s="14"/>
+      <c r="Z34" s="14"/>
+      <c r="AA34" s="18">
+        <v>64</v>
+      </c>
+      <c r="AB34" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC34" s="19"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="2" t="s">
         <v>36</v>
       </c>
@@ -3021,31 +3480,38 @@
         <v>75</v>
       </c>
       <c r="E35" s="3"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
-      <c r="R35" s="9"/>
-      <c r="S35" s="9"/>
-      <c r="T35" s="9"/>
-      <c r="U35" s="12"/>
-      <c r="V35" s="12"/>
-      <c r="W35" s="12"/>
-      <c r="X35" s="15"/>
-      <c r="Y35" s="15"/>
-      <c r="Z35" s="15"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="8"/>
+      <c r="T35" s="8"/>
+      <c r="U35" s="11"/>
+      <c r="V35" s="11"/>
+      <c r="W35" s="11"/>
+      <c r="X35" s="14"/>
+      <c r="Y35" s="14"/>
+      <c r="Z35" s="14"/>
+      <c r="AA35" s="18">
+        <v>65</v>
+      </c>
+      <c r="AB35" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="AC35" s="19"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
       <c r="C36" s="2" t="s">
         <v>37</v>
       </c>
@@ -3053,31 +3519,31 @@
         <v>76</v>
       </c>
       <c r="E36" s="3"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="9"/>
-      <c r="R36" s="9"/>
-      <c r="S36" s="9"/>
-      <c r="T36" s="9"/>
-      <c r="U36" s="12"/>
-      <c r="V36" s="12"/>
-      <c r="W36" s="12"/>
-      <c r="X36" s="15"/>
-      <c r="Y36" s="15"/>
-      <c r="Z36" s="15"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+      <c r="T36" s="8"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11"/>
+      <c r="W36" s="11"/>
+      <c r="X36" s="14"/>
+      <c r="Y36" s="14"/>
+      <c r="Z36" s="14"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="9"/>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="2" t="s">
         <v>38</v>
       </c>
@@ -3085,27 +3551,27 @@
         <v>77</v>
       </c>
       <c r="E37" s="3"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
-      <c r="O37" s="9"/>
-      <c r="P37" s="9"/>
-      <c r="Q37" s="9"/>
-      <c r="R37" s="9"/>
-      <c r="S37" s="9"/>
-      <c r="T37" s="9"/>
-      <c r="U37" s="12"/>
-      <c r="V37" s="12"/>
-      <c r="W37" s="12"/>
-      <c r="X37" s="15"/>
-      <c r="Y37" s="15"/>
-      <c r="Z37" s="15"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="8"/>
+      <c r="U37" s="11"/>
+      <c r="V37" s="11"/>
+      <c r="W37" s="11"/>
+      <c r="X37" s="14"/>
+      <c r="Y37" s="14"/>
+      <c r="Z37" s="14"/>
     </row>
   </sheetData>
   <dataValidations count="20">
@@ -3116,9 +3582,7 @@
     <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Name must be less than 20 characters_x000a_" sqref="B7 B2" xr:uid="{91D9CADE-1361-894F-81E5-FC375AB75B27}">
       <formula1>19</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" sqref="B6" xr:uid="{78435723-4E53-3A4B-84FA-56E94593458F}">
-      <formula1>9</formula1>
-    </dataValidation>
+    <dataValidation operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" sqref="B6" xr:uid="{78435723-4E53-3A4B-84FA-56E94593458F}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Please input either 'M' or 'F'" sqref="B5" xr:uid="{BC652F4B-BEAA-BE40-980A-D8D5DBBFFAAC}">
       <formula1>"M,F"</formula1>
     </dataValidation>
@@ -3144,9 +3608,7 @@
       <formula1>0</formula1>
       <formula2>4</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Enter DOB in format DD.MM.YY" sqref="B9" xr:uid="{8677C5A0-DDA8-5744-BD30-25679193FB92}">
-      <formula1>9</formula1>
-    </dataValidation>
+    <dataValidation operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Enter DOB in format DD.MM.YY" sqref="B9" xr:uid="{8677C5A0-DDA8-5744-BD30-25679193FB92}"/>
     <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Max length 19 characters" sqref="B3" xr:uid="{F302C943-075C-5A46-BAE7-3AB0FDA9DACF}">
       <formula1>19</formula1>
     </dataValidation>
@@ -3168,16 +3630,16 @@
       <formula1>0</formula1>
       <formula2>3</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input a number between 0 and 4" sqref="Z2:Z7 Z9 Z21:Z23 Z20 Z8" xr:uid="{F7AEEDA1-C641-A946-B2D6-50CF8F25AB41}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input a number between 0 and 4" sqref="Z20:Z23 Z2:Z9 T2:T21" xr:uid="{F7AEEDA1-C641-A946-B2D6-50CF8F25AB41}">
       <formula1>0</formula1>
       <formula2>4</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input either 'Y' or 'N'" sqref="Z10:Z19" xr:uid="{C45CB5A2-312A-9349-BC4A-AA78049DC6D5}">
       <formula1>"Y, N"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input a number between 0 and 4" sqref="T2:T21" xr:uid="{A7F9FF7C-FF09-EC46-BFD7-DDA6C142E68D}">
-      <formula1>0</formula1>
-      <formula2>4</formula2>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input a number between 1 and 5." sqref="AC2:AC35" xr:uid="{C5C022E8-27A2-0343-A204-FA487880999E}">
+      <formula1>1</formula1>
+      <formula2>5</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
percentages added to WHODAS files, and CASP added to files
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksnelling/Desktop/form-creator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1095B92-7E7D-2E41-B178-82B9ACED03E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033CF4D1-05F7-3347-A36F-319B037C6DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18040" yWindow="880" windowWidth="17960" windowHeight="20420" xr2:uid="{5B803FEE-CBC5-CD4B-BFE8-7DF0DABD6B40}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="279">
   <si>
     <t>age</t>
   </si>
@@ -429,9 +429,6 @@
   </si>
   <si>
     <t>H</t>
-  </si>
-  <si>
-    <t>ndis_no</t>
   </si>
   <si>
     <t>BBS</t>
@@ -1089,7 +1086,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1125,11 +1122,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1153,9 +1198,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1163,9 +1205,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1195,8 +1234,51 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1538,10 +1620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45B32DC-4C24-CA4A-AFD2-C2BFFA6D046C}">
-  <dimension ref="A1:AC37"/>
+  <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1551,27 +1633,27 @@
     <col min="3" max="3" width="15.1640625" customWidth="1"/>
     <col min="4" max="4" width="52.83203125" customWidth="1"/>
     <col min="5" max="5" width="21.1640625" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="39.5" customWidth="1"/>
-    <col min="8" max="8" width="19.1640625" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="74.5" style="11" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" style="11" customWidth="1"/>
     <col min="9" max="9" width="19.6640625" customWidth="1"/>
     <col min="10" max="10" width="59.1640625" customWidth="1"/>
     <col min="12" max="12" width="13.1640625" customWidth="1"/>
     <col min="13" max="13" width="71.1640625" customWidth="1"/>
     <col min="14" max="14" width="18" customWidth="1"/>
     <col min="15" max="15" width="10.83203125" customWidth="1"/>
-    <col min="16" max="16" width="63.1640625" customWidth="1"/>
+    <col min="16" max="16" width="67" customWidth="1"/>
     <col min="17" max="17" width="24.6640625" customWidth="1"/>
-    <col min="19" max="19" width="45.33203125" customWidth="1"/>
+    <col min="19" max="19" width="55.33203125" customWidth="1"/>
     <col min="21" max="21" width="16.83203125" customWidth="1"/>
     <col min="22" max="22" width="55.5" customWidth="1"/>
-    <col min="24" max="24" width="10.83203125" style="13"/>
-    <col min="25" max="25" width="49.33203125" style="13" customWidth="1"/>
-    <col min="26" max="26" width="18.5" style="13" customWidth="1"/>
-    <col min="27" max="27" width="14.6640625" style="13" customWidth="1"/>
-    <col min="28" max="28" width="75.83203125" style="13" customWidth="1"/>
-    <col min="29" max="29" width="21.33203125" style="13" customWidth="1"/>
-    <col min="30" max="16384" width="10.83203125" style="13"/>
+    <col min="24" max="24" width="16.33203125" style="11" customWidth="1"/>
+    <col min="25" max="25" width="58.6640625" style="11" customWidth="1"/>
+    <col min="26" max="26" width="18.5" style="11" customWidth="1"/>
+    <col min="27" max="27" width="14.6640625" style="11" customWidth="1"/>
+    <col min="28" max="28" width="50.6640625" style="11" customWidth="1"/>
+    <col min="29" max="29" width="21.33203125" style="11" customWidth="1"/>
+    <col min="33" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
@@ -1590,82 +1672,82 @@
       <c r="E1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>104</v>
+        <v>41</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>213</v>
+        <v>172</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Z1" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="AA1" s="17" t="s">
-        <v>270</v>
-      </c>
-      <c r="AB1" s="17" t="s">
+      <c r="Z1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AC1" s="17" t="s">
-        <v>271</v>
+      <c r="AC1" s="13" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
@@ -1676,65 +1758,65 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="4">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H2" s="3"/>
+        <v>236</v>
+      </c>
+      <c r="H2" s="5"/>
       <c r="I2" s="4">
         <v>1</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="4">
+        <v>1</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="4" t="s">
+      <c r="N2" s="5"/>
+      <c r="O2" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="N2" s="5"/>
-      <c r="O2" s="4">
-        <v>1</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>134</v>
+      <c r="P2" s="6" t="s">
+        <v>271</v>
       </c>
       <c r="Q2" s="5"/>
       <c r="R2" s="4">
         <v>1</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="T2" s="5"/>
-      <c r="U2" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>207</v>
+      <c r="U2" s="4">
+        <v>1</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>150</v>
       </c>
       <c r="W2" s="5"/>
-      <c r="X2" s="4">
+      <c r="X2" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="4">
         <v>1</v>
       </c>
-      <c r="Y2" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="4">
-        <v>11</v>
-      </c>
       <c r="AB2" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="AC2" s="5"/>
+        <v>214</v>
+      </c>
+      <c r="AC2" s="14"/>
     </row>
     <row r="3" spans="1:29" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="2" t="s">
@@ -1745,61 +1827,61 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="4">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H3" s="3"/>
+        <v>237</v>
+      </c>
+      <c r="H3" s="5"/>
       <c r="I3" s="4">
         <v>2</v>
       </c>
       <c r="J3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="4">
+        <v>2</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="4" t="s">
+      <c r="N3" s="5"/>
+      <c r="O3" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="4">
-        <v>2</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>135</v>
+      <c r="P3" s="6" t="s">
+        <v>272</v>
       </c>
       <c r="Q3" s="5"/>
       <c r="R3" s="4">
         <v>2</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="T3" s="5"/>
-      <c r="U3" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>191</v>
+      <c r="U3" s="4">
+        <v>2</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="W3" s="5"/>
-      <c r="X3" s="4">
+      <c r="X3" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="4">
         <v>2</v>
       </c>
-      <c r="Y3" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="Z3" s="16"/>
-      <c r="AA3" s="4">
-        <v>12</v>
-      </c>
       <c r="AB3" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="AC3" s="5"/>
+        <v>215</v>
+      </c>
+      <c r="AC3" s="14"/>
     </row>
     <row r="4" spans="1:29" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -1814,61 +1896,61 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="4">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" s="3"/>
+        <v>238</v>
+      </c>
+      <c r="H4" s="5"/>
       <c r="I4" s="4">
         <v>3</v>
       </c>
       <c r="J4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="4">
+        <v>3</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="4" t="s">
+      <c r="N4" s="5"/>
+      <c r="O4" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="M4" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="N4" s="5"/>
-      <c r="O4" s="4">
-        <v>3</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>136</v>
+      <c r="P4" s="6" t="s">
+        <v>273</v>
       </c>
       <c r="Q4" s="5"/>
       <c r="R4" s="4">
         <v>3</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="T4" s="5"/>
-      <c r="U4" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="V4" s="6" t="s">
-        <v>192</v>
+      <c r="U4" s="4">
+        <v>3</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="W4" s="5"/>
-      <c r="X4" s="4">
+      <c r="X4" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="4">
         <v>3</v>
       </c>
-      <c r="Y4" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="4">
-        <v>13</v>
-      </c>
       <c r="AB4" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="AC4" s="5"/>
+        <v>216</v>
+      </c>
+      <c r="AC4" s="14"/>
     </row>
     <row r="5" spans="1:29" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -1883,67 +1965,67 @@
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="4">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H5" s="3"/>
+        <v>239</v>
+      </c>
+      <c r="H5" s="5"/>
       <c r="I5" s="4">
         <v>4</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="4">
+        <v>4</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="4" t="s">
+      <c r="N5" s="5"/>
+      <c r="O5" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="M5" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="N5" s="5"/>
-      <c r="O5" s="4">
-        <v>4</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>137</v>
+      <c r="P5" s="6" t="s">
+        <v>274</v>
       </c>
       <c r="Q5" s="5"/>
       <c r="R5" s="4">
         <v>4</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="T5" s="5"/>
-      <c r="U5" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>193</v>
+      <c r="U5" s="4">
+        <v>4</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>153</v>
       </c>
       <c r="W5" s="5"/>
-      <c r="X5" s="4">
+      <c r="X5" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="Y5" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="4">
         <v>4</v>
       </c>
-      <c r="Y5" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="Z5" s="16"/>
-      <c r="AA5" s="4">
-        <v>14</v>
-      </c>
       <c r="AB5" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="AC5" s="5"/>
+        <v>217</v>
+      </c>
+      <c r="AC5" s="14"/>
     </row>
     <row r="6" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="20"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1952,61 +2034,61 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="4">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H6" s="3"/>
+        <v>240</v>
+      </c>
+      <c r="H6" s="5"/>
       <c r="I6" s="4">
         <v>5</v>
       </c>
       <c r="J6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="4">
+        <v>5</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="4" t="s">
+      <c r="N6" s="5"/>
+      <c r="O6" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="M6" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="N6" s="5"/>
-      <c r="O6" s="4">
-        <v>5</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>138</v>
+      <c r="P6" s="6" t="s">
+        <v>275</v>
       </c>
       <c r="Q6" s="5"/>
       <c r="R6" s="4">
         <v>5</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="T6" s="5"/>
-      <c r="U6" s="4" t="s">
-        <v>179</v>
+      <c r="U6" s="4">
+        <v>5</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>194</v>
+        <v>154</v>
       </c>
       <c r="W6" s="5"/>
-      <c r="X6" s="4">
+      <c r="X6" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="4">
         <v>5</v>
       </c>
-      <c r="Y6" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="Z6" s="16"/>
-      <c r="AA6" s="4">
-        <v>15</v>
-      </c>
       <c r="AB6" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="AC6" s="5"/>
+        <v>218</v>
+      </c>
+      <c r="AC6" s="14"/>
     </row>
     <row r="7" spans="1:29" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -2021,67 +2103,67 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="4">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="3"/>
+        <v>241</v>
+      </c>
+      <c r="H7" s="5"/>
       <c r="I7" s="4">
         <v>6</v>
       </c>
       <c r="J7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="4">
+        <v>6</v>
+      </c>
+      <c r="M7" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="4" t="s">
+      <c r="N7" s="5"/>
+      <c r="O7" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="M7" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="N7" s="5"/>
-      <c r="O7" s="4">
-        <v>6</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>139</v>
+      <c r="P7" s="6" t="s">
+        <v>276</v>
       </c>
       <c r="Q7" s="5"/>
       <c r="R7" s="4">
         <v>6</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="T7" s="5"/>
-      <c r="U7" s="4" t="s">
-        <v>180</v>
+      <c r="U7" s="4">
+        <v>6</v>
       </c>
       <c r="V7" s="4" t="s">
-        <v>195</v>
+        <v>155</v>
       </c>
       <c r="W7" s="5"/>
-      <c r="X7" s="4">
+      <c r="X7" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y7" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="4">
         <v>6</v>
       </c>
-      <c r="Y7" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="Z7" s="16"/>
-      <c r="AA7" s="4">
-        <v>16</v>
-      </c>
       <c r="AB7" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="AC7" s="5"/>
+        <v>219</v>
+      </c>
+      <c r="AC7" s="14"/>
     </row>
-    <row r="8" spans="1:29" ht="68" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B8" s="5"/>
+    <row r="8" spans="1:29" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="21"/>
       <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
@@ -2090,68 +2172,64 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="4">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" s="3"/>
+        <v>242</v>
+      </c>
+      <c r="H8" s="5"/>
       <c r="I8" s="4">
         <v>7</v>
       </c>
       <c r="J8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="4">
+        <v>7</v>
+      </c>
+      <c r="M8" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="4" t="s">
+      <c r="N8" s="5"/>
+      <c r="O8" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="M8" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="N8" s="5"/>
-      <c r="O8" s="4">
-        <v>7</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>140</v>
+      <c r="P8" s="6" t="s">
+        <v>277</v>
       </c>
       <c r="Q8" s="5"/>
       <c r="R8" s="4">
         <v>7</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="T8" s="5"/>
-      <c r="U8" s="4" t="s">
-        <v>181</v>
+      <c r="U8" s="4">
+        <v>7</v>
       </c>
       <c r="V8" s="4" t="s">
-        <v>196</v>
+        <v>156</v>
       </c>
       <c r="W8" s="5"/>
-      <c r="X8" s="4">
+      <c r="X8" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y8" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="4">
         <v>7</v>
       </c>
-      <c r="Y8" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="Z8" s="16"/>
-      <c r="AA8" s="4">
-        <v>21</v>
-      </c>
       <c r="AB8" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="AC8" s="5"/>
+        <v>220</v>
+      </c>
+      <c r="AC8" s="14"/>
     </row>
-    <row r="9" spans="1:29" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="2" t="s">
+    <row r="9" spans="1:29" ht="85" x14ac:dyDescent="0.2">
+      <c r="C9" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -2159,66 +2237,66 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="4">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H9" s="3"/>
+        <v>243</v>
+      </c>
+      <c r="H9" s="5"/>
       <c r="I9" s="4">
         <v>8</v>
       </c>
       <c r="J9" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="4">
+        <v>8</v>
+      </c>
+      <c r="M9" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="4" t="s">
+      <c r="N9" s="5"/>
+      <c r="O9" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="M9" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="N9" s="5"/>
-      <c r="O9" s="4">
-        <v>8</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q9" s="5"/>
+      <c r="P9" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q9" s="26"/>
       <c r="R9" s="4">
         <v>8</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="T9" s="5"/>
-      <c r="U9" s="4" t="s">
-        <v>182</v>
+      <c r="U9" s="4">
+        <v>8</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>197</v>
+        <v>157</v>
       </c>
       <c r="W9" s="5"/>
-      <c r="X9" s="4">
+      <c r="X9" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y9" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="4">
         <v>8</v>
       </c>
-      <c r="Y9" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="Z9" s="16"/>
-      <c r="AA9" s="4">
-        <v>22</v>
-      </c>
       <c r="AB9" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="AC9" s="5"/>
+        <v>235</v>
+      </c>
+      <c r="AC9" s="14"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="2" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="19" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -2226,62 +2304,62 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="4">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="H10" s="3"/>
+        <v>244</v>
+      </c>
+      <c r="H10" s="5"/>
       <c r="I10" s="4">
         <v>9</v>
       </c>
       <c r="J10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="4">
+        <v>9</v>
+      </c>
+      <c r="M10" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="4">
+      <c r="N10" s="14"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="28">
         <v>9</v>
       </c>
-      <c r="P10" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="4">
+      <c r="S10" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="T10" s="5"/>
+      <c r="U10" s="4">
         <v>9</v>
       </c>
-      <c r="S10" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="T10" s="5"/>
-      <c r="U10" s="4" t="s">
-        <v>138</v>
-      </c>
       <c r="V10" s="4" t="s">
-        <v>198</v>
+        <v>158</v>
       </c>
       <c r="W10" s="5"/>
       <c r="X10" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y10" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="Y10" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="Z10" s="16"/>
-      <c r="AA10" s="4">
-        <v>23</v>
-      </c>
       <c r="AB10" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="AC10" s="5"/>
+        <v>225</v>
+      </c>
+      <c r="AC10" s="14"/>
     </row>
     <row r="11" spans="1:29" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="2" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -2289,62 +2367,62 @@
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="4">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H11" s="3"/>
+        <v>245</v>
+      </c>
+      <c r="H11" s="5"/>
       <c r="I11" s="4">
         <v>10</v>
       </c>
       <c r="J11" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="4">
+        <v>10</v>
+      </c>
+      <c r="M11" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="4">
+      <c r="N11" s="14"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="28">
         <v>10</v>
       </c>
-      <c r="P11" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="4">
+      <c r="S11" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="T11" s="5"/>
+      <c r="U11" s="4">
         <v>10</v>
       </c>
-      <c r="S11" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="T11" s="5"/>
-      <c r="U11" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="V11" s="6" t="s">
-        <v>199</v>
+      <c r="V11" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="W11" s="5"/>
       <c r="X11" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="Y11" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="Y11" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="Z11" s="16"/>
-      <c r="AA11" s="4">
-        <v>24</v>
-      </c>
       <c r="AB11" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="AC11" s="5"/>
+        <v>226</v>
+      </c>
+      <c r="AC11" s="14"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="2" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="19" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -2352,62 +2430,62 @@
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="4">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="H12" s="3"/>
+        <v>246</v>
+      </c>
+      <c r="H12" s="5"/>
       <c r="I12" s="4">
         <v>11</v>
       </c>
       <c r="J12" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" s="3"/>
+      <c r="L12" s="4">
+        <v>11</v>
+      </c>
+      <c r="M12" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="4">
+      <c r="N12" s="14"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="28">
         <v>11</v>
       </c>
-      <c r="P12" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="4">
+      <c r="S12" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="T12" s="5"/>
+      <c r="U12" s="4">
         <v>11</v>
       </c>
-      <c r="S12" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="T12" s="5"/>
-      <c r="U12" s="4" t="s">
-        <v>184</v>
-      </c>
       <c r="V12" s="4" t="s">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="W12" s="5"/>
       <c r="X12" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y12" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="Y12" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="Z12" s="16"/>
-      <c r="AA12" s="4">
-        <v>25</v>
-      </c>
       <c r="AB12" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="AC12" s="5"/>
+        <v>229</v>
+      </c>
+      <c r="AC12" s="14"/>
     </row>
-    <row r="13" spans="1:29" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="2" t="s">
+    <row r="13" spans="1:29" ht="204" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="19" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -2415,62 +2493,62 @@
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="4">
-        <v>12</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="H13" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="H13" s="5"/>
       <c r="I13" s="4">
         <v>12</v>
       </c>
       <c r="J13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K13" s="3"/>
+      <c r="L13" s="4">
+        <v>12</v>
+      </c>
+      <c r="M13" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="4">
+      <c r="N13" s="14"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="28">
         <v>12</v>
       </c>
-      <c r="P13" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="4">
+      <c r="S13" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="T13" s="5"/>
+      <c r="U13" s="4">
         <v>12</v>
       </c>
-      <c r="S13" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="T13" s="5"/>
-      <c r="U13" s="4" t="s">
-        <v>185</v>
-      </c>
       <c r="V13" s="4" t="s">
-        <v>201</v>
+        <v>161</v>
       </c>
       <c r="W13" s="5"/>
       <c r="X13" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="Y13" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="Y13" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="Z13" s="16"/>
-      <c r="AA13" s="4">
-        <v>31</v>
-      </c>
-      <c r="AB13" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="AC13" s="5"/>
+      <c r="AB13" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="AC13" s="14"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="2" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="19" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -2478,62 +2556,62 @@
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="4">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H14" s="3"/>
+        <v>248</v>
+      </c>
+      <c r="H14" s="5"/>
       <c r="I14" s="4">
         <v>13</v>
       </c>
       <c r="J14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="4">
+        <v>13</v>
+      </c>
+      <c r="M14" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="K14" s="5"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="4">
+      <c r="N14" s="14"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="28">
         <v>13</v>
       </c>
-      <c r="P14" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="4">
+      <c r="S14" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="T14" s="5"/>
+      <c r="U14" s="4">
         <v>13</v>
       </c>
-      <c r="S14" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="T14" s="5"/>
-      <c r="U14" s="4" t="s">
-        <v>186</v>
-      </c>
       <c r="V14" s="4" t="s">
-        <v>202</v>
+        <v>162</v>
       </c>
       <c r="W14" s="5"/>
       <c r="X14" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y14" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="Y14" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="Z14" s="16"/>
-      <c r="AA14" s="4">
-        <v>32</v>
-      </c>
       <c r="AB14" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="AC14" s="5"/>
+        <v>231</v>
+      </c>
+      <c r="AC14" s="14"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="2" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="19" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -2541,62 +2619,62 @@
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="4">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H15" s="3"/>
+        <v>249</v>
+      </c>
+      <c r="H15" s="5"/>
       <c r="I15" s="4">
         <v>14</v>
       </c>
       <c r="J15" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K15" s="3"/>
+      <c r="L15" s="4">
+        <v>14</v>
+      </c>
+      <c r="M15" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="K15" s="5"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="4">
+      <c r="N15" s="14"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="30">
         <v>14</v>
       </c>
-      <c r="P15" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="4">
+      <c r="S15" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="T15" s="26"/>
+      <c r="U15" s="4">
         <v>14</v>
       </c>
-      <c r="S15" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="T15" s="5"/>
-      <c r="U15" s="4" t="s">
-        <v>187</v>
-      </c>
       <c r="V15" s="4" t="s">
-        <v>203</v>
+        <v>163</v>
       </c>
       <c r="W15" s="5"/>
       <c r="X15" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y15" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="Y15" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="Z15" s="16"/>
-      <c r="AA15" s="4">
-        <v>33</v>
-      </c>
       <c r="AB15" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="AC15" s="5"/>
+        <v>232</v>
+      </c>
+      <c r="AC15" s="14"/>
     </row>
     <row r="16" spans="1:29" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="2" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="19" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -2604,58 +2682,58 @@
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="4">
-        <v>15</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" s="9"/>
+        <v>34</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="H16" s="5"/>
       <c r="I16" s="4">
         <v>15</v>
       </c>
       <c r="J16" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K16" s="8"/>
+      <c r="L16" s="4">
+        <v>15</v>
+      </c>
+      <c r="M16" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="4">
+      <c r="N16" s="14"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="28">
         <v>15</v>
       </c>
-      <c r="S16" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="T16" s="5"/>
-      <c r="U16" s="4" t="s">
-        <v>188</v>
-      </c>
       <c r="V16" s="4" t="s">
-        <v>204</v>
+        <v>164</v>
       </c>
       <c r="W16" s="5"/>
       <c r="X16" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Y16" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="Y16" s="4" t="s">
+      <c r="AB16" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="Z16" s="16"/>
-      <c r="AA16" s="4">
-        <v>34</v>
-      </c>
-      <c r="AB16" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="AC16" s="5"/>
+      <c r="AC16" s="14"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="2" t="s">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="19" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -2663,58 +2741,58 @@
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="4">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="H17" s="10"/>
+        <v>251</v>
+      </c>
+      <c r="H17" s="5"/>
       <c r="I17" s="4">
         <v>16</v>
       </c>
       <c r="J17" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K17" s="9"/>
+      <c r="L17" s="20">
+        <v>16</v>
+      </c>
+      <c r="M17" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="4">
+      <c r="N17" s="27"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="28">
         <v>16</v>
       </c>
-      <c r="S17" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="T17" s="5"/>
-      <c r="U17" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="V17" s="4" t="s">
-        <v>205</v>
+        <v>165</v>
       </c>
       <c r="W17" s="5"/>
       <c r="X17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y17" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="Y17" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="Z17" s="16"/>
-      <c r="AA17" s="4">
-        <v>41</v>
-      </c>
       <c r="AB17" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="AC17" s="5"/>
+        <v>233</v>
+      </c>
+      <c r="AC17" s="14"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="2" t="s">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="19" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -2722,54 +2800,54 @@
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="4">
+        <v>42</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="H18" s="5"/>
+      <c r="I18" s="4">
         <v>17</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="J18" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="4">
+      <c r="K18" s="23"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="28">
         <v>17</v>
       </c>
-      <c r="S18" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="T18" s="5"/>
-      <c r="U18" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="V18" s="12" t="s">
-        <v>206</v>
+      <c r="V18" s="4" t="s">
+        <v>166</v>
       </c>
       <c r="W18" s="5"/>
       <c r="X18" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="Y18" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="Z18" s="16"/>
-      <c r="AA18" s="4">
-        <v>42</v>
+        <v>87</v>
+      </c>
+      <c r="Y18" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="4" t="s">
+        <v>227</v>
       </c>
       <c r="AB18" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="AC18" s="5"/>
+        <v>234</v>
+      </c>
+      <c r="AC18" s="14"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="2" t="s">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="4" t="s">
@@ -2777,54 +2855,54 @@
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="4">
+        <v>43</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="4">
         <v>18</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="J19" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="4">
+      <c r="K19" s="23"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="28">
         <v>18</v>
       </c>
-      <c r="S19" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="T19" s="5"/>
-      <c r="U19" s="4" t="s">
+      <c r="V19" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="W19" s="5"/>
+      <c r="X19" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="Y19" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="V19" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="W19" s="5"/>
-      <c r="X19" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="Y19" s="4" t="s">
+      <c r="Z19" s="26"/>
+      <c r="AA19" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="AB19" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="Z19" s="16"/>
-      <c r="AA19" s="4">
-        <v>43</v>
-      </c>
-      <c r="AB19" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="AC19" s="5"/>
+      <c r="AC19" s="14"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="2" t="s">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="19" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="4" t="s">
@@ -2832,50 +2910,50 @@
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="4">
+        <v>44</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="4">
         <v>19</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="J20" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="4">
+      <c r="K20" s="23"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="28">
         <v>19</v>
       </c>
-      <c r="S20" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="T20" s="5"/>
-      <c r="U20" s="11"/>
-      <c r="V20" s="11"/>
-      <c r="W20" s="11"/>
-      <c r="X20" s="4">
+      <c r="V20" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="W20" s="14"/>
+      <c r="X20" s="32"/>
+      <c r="Y20" s="32"/>
+      <c r="Z20" s="32"/>
+      <c r="AA20" s="28">
         <v>9</v>
       </c>
-      <c r="Y20" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="Z20" s="16"/>
-      <c r="AA20" s="4">
-        <v>44</v>
-      </c>
       <c r="AB20" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC20" s="5"/>
+        <v>221</v>
+      </c>
+      <c r="AC20" s="14"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="2" t="s">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="4" t="s">
@@ -2883,50 +2961,50 @@
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="4">
+        <v>45</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="4">
         <v>20</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="J21" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="4">
+      <c r="K21" s="23"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="30">
         <v>20</v>
       </c>
-      <c r="S21" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="T21" s="5"/>
-      <c r="U21" s="11"/>
-      <c r="V21" s="11"/>
-      <c r="W21" s="11"/>
-      <c r="X21" s="4">
+      <c r="V21" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="W21" s="27"/>
+      <c r="X21" s="32"/>
+      <c r="Y21" s="32"/>
+      <c r="Z21" s="32"/>
+      <c r="AA21" s="28">
         <v>10</v>
       </c>
-      <c r="Y21" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z21" s="16"/>
-      <c r="AA21" s="4">
-        <v>45</v>
-      </c>
       <c r="AB21" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="AC21" s="5"/>
+        <v>222</v>
+      </c>
+      <c r="AC21" s="14"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="2" t="s">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="19" t="s">
         <v>23</v>
       </c>
       <c r="D22" s="4" t="s">
@@ -2934,46 +3012,46 @@
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="4">
+        <v>51</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="H22" s="5"/>
+      <c r="I22" s="4">
         <v>21</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="J22" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="8"/>
-      <c r="U22" s="11"/>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="4">
+      <c r="K22" s="22"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="12"/>
+      <c r="X22" s="32"/>
+      <c r="Y22" s="32"/>
+      <c r="Z22" s="32"/>
+      <c r="AA22" s="28">
         <v>11</v>
       </c>
-      <c r="Y22" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="Z22" s="16"/>
-      <c r="AA22" s="4">
-        <v>51</v>
-      </c>
       <c r="AB22" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="AC22" s="5"/>
+        <v>223</v>
+      </c>
+      <c r="AC22" s="14"/>
     </row>
     <row r="23" spans="1:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="2" t="s">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="19" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="4" t="s">
@@ -2981,600 +3059,594 @@
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="4">
+        <v>52</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="H23" s="5"/>
+      <c r="I23" s="4">
         <v>22</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="J23" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H23" s="9"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
-      <c r="T23" s="8"/>
-      <c r="U23" s="11"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="4">
+      <c r="K23" s="24"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="12"/>
+      <c r="X23" s="32"/>
+      <c r="Y23" s="32"/>
+      <c r="Z23" s="32"/>
+      <c r="AA23" s="28">
         <v>12</v>
       </c>
-      <c r="Y23" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="Z23" s="16"/>
-      <c r="AA23" s="4">
-        <v>52</v>
-      </c>
       <c r="AB23" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="AC23" s="5"/>
+        <v>224</v>
+      </c>
+      <c r="AC23" s="14"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="2" t="s">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="19" t="s">
         <v>25</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>69</v>
       </c>
       <c r="E24" s="3"/>
-      <c r="F24" s="4">
+      <c r="F24" s="16">
+        <v>53</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="H24" s="17"/>
+      <c r="I24" s="4">
         <v>23</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="J24" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
-      <c r="T24" s="8"/>
-      <c r="U24" s="11"/>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="14"/>
-      <c r="Y24" s="14"/>
-      <c r="Z24" s="14"/>
-      <c r="AA24" s="18">
-        <v>53</v>
-      </c>
-      <c r="AB24" s="18" t="s">
-        <v>258</v>
-      </c>
-      <c r="AC24" s="19"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="12"/>
+      <c r="T24" s="12"/>
+      <c r="U24" s="12"/>
+      <c r="V24" s="12"/>
+      <c r="W24" s="12"/>
+      <c r="X24" s="32"/>
+      <c r="Y24" s="32"/>
+      <c r="Z24" s="32"/>
+      <c r="AA24" s="12"/>
+      <c r="AB24" s="12"/>
+      <c r="AC24" s="12"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="2" t="s">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="19" t="s">
         <v>26</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>70</v>
       </c>
       <c r="E25" s="3"/>
-      <c r="F25" s="4">
+      <c r="F25" s="16">
+        <v>54</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="H25" s="17"/>
+      <c r="I25" s="4">
         <v>24</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="J25" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="H25" s="10"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="14"/>
-      <c r="Y25" s="14"/>
-      <c r="Z25" s="14"/>
-      <c r="AA25" s="18">
-        <v>54</v>
-      </c>
-      <c r="AB25" s="18" t="s">
-        <v>259</v>
-      </c>
-      <c r="AC25" s="19"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
+      <c r="U25" s="12"/>
+      <c r="V25" s="12"/>
+      <c r="W25" s="12"/>
+      <c r="X25" s="32"/>
+      <c r="Y25" s="32"/>
+      <c r="Z25" s="32"/>
+      <c r="AA25" s="12"/>
+      <c r="AB25" s="12"/>
+      <c r="AC25" s="12"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="2" t="s">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="19" t="s">
         <v>27</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E26" s="3"/>
-      <c r="F26" s="4">
+      <c r="F26" s="16">
+        <v>55</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="H26" s="17"/>
+      <c r="I26" s="4">
         <v>25</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="J26" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="H26" s="10"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
-      <c r="T26" s="8"/>
-      <c r="U26" s="11"/>
-      <c r="V26" s="11"/>
-      <c r="W26" s="11"/>
-      <c r="X26" s="14"/>
-      <c r="Y26" s="14"/>
-      <c r="Z26" s="14"/>
-      <c r="AA26" s="18">
-        <v>55</v>
-      </c>
-      <c r="AB26" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="AC26" s="19"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+      <c r="V26" s="12"/>
+      <c r="W26" s="12"/>
+      <c r="X26" s="32"/>
+      <c r="Y26" s="32"/>
+      <c r="Z26" s="32"/>
+      <c r="AA26" s="12"/>
+      <c r="AB26" s="12"/>
+      <c r="AC26" s="12"/>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="2" t="s">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E27" s="3"/>
-      <c r="F27" s="4">
+      <c r="F27" s="16">
+        <v>56</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="H27" s="17"/>
+      <c r="I27" s="4">
         <v>26</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="J27" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="H27" s="10"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="8"/>
-      <c r="U27" s="11"/>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-      <c r="X27" s="14"/>
-      <c r="Y27" s="14"/>
-      <c r="Z27" s="14"/>
-      <c r="AA27" s="18">
-        <v>56</v>
-      </c>
-      <c r="AB27" s="18" t="s">
-        <v>269</v>
-      </c>
-      <c r="AC27" s="19"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="12"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="32"/>
+      <c r="Y27" s="32"/>
+      <c r="Z27" s="32"/>
+      <c r="AA27" s="12"/>
+      <c r="AB27" s="12"/>
+      <c r="AC27" s="12"/>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="2" t="s">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E28" s="3"/>
-      <c r="F28" s="4">
+      <c r="F28" s="16">
+        <v>57</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="H28" s="17"/>
+      <c r="I28" s="4">
         <v>27</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="J28" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="H28" s="10"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="11"/>
-      <c r="V28" s="11"/>
-      <c r="W28" s="11"/>
-      <c r="X28" s="14"/>
-      <c r="Y28" s="14"/>
-      <c r="Z28" s="14"/>
-      <c r="AA28" s="18">
-        <v>57</v>
-      </c>
-      <c r="AB28" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="AC28" s="19"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="12"/>
+      <c r="U28" s="12"/>
+      <c r="V28" s="12"/>
+      <c r="W28" s="12"/>
+      <c r="X28" s="32"/>
+      <c r="Y28" s="32"/>
+      <c r="Z28" s="32"/>
+      <c r="AA28" s="12"/>
+      <c r="AB28" s="12"/>
+      <c r="AC28" s="12"/>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="2" t="s">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="19" t="s">
         <v>30</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E29" s="3"/>
-      <c r="F29" s="4">
+      <c r="F29" s="16">
+        <v>58</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="H29" s="17"/>
+      <c r="I29" s="20">
         <v>28</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="J29" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="H29" s="3"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
-      <c r="U29" s="11"/>
-      <c r="V29" s="11"/>
-      <c r="W29" s="11"/>
-      <c r="X29" s="14"/>
-      <c r="Y29" s="14"/>
-      <c r="Z29" s="14"/>
-      <c r="AA29" s="18">
-        <v>58</v>
-      </c>
-      <c r="AB29" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="AC29" s="19"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="12"/>
+      <c r="U29" s="12"/>
+      <c r="V29" s="12"/>
+      <c r="W29" s="12"/>
+      <c r="X29" s="32"/>
+      <c r="Y29" s="32"/>
+      <c r="Z29" s="32"/>
+      <c r="AA29" s="12"/>
+      <c r="AB29" s="12"/>
+      <c r="AC29" s="12"/>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="2" t="s">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="19" t="s">
         <v>31</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="8"/>
-      <c r="U30" s="11"/>
-      <c r="V30" s="11"/>
-      <c r="W30" s="11"/>
-      <c r="X30" s="14"/>
-      <c r="Y30" s="14"/>
-      <c r="Z30" s="14"/>
-      <c r="AA30" s="18">
+        <v>210</v>
+      </c>
+      <c r="E30" s="22"/>
+      <c r="F30" s="16">
         <v>59</v>
       </c>
-      <c r="AB30" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="AC30" s="19"/>
+      <c r="G30" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="H30" s="17"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="12"/>
+      <c r="W30" s="12"/>
+      <c r="X30" s="32"/>
+      <c r="Y30" s="32"/>
+      <c r="Z30" s="32"/>
+      <c r="AA30" s="12"/>
+      <c r="AB30" s="12"/>
+      <c r="AC30" s="12"/>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="2" t="s">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="19" t="s">
         <v>32</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
-      <c r="U31" s="11"/>
-      <c r="V31" s="11"/>
-      <c r="W31" s="11"/>
-      <c r="X31" s="14"/>
-      <c r="Y31" s="14"/>
-      <c r="Z31" s="14"/>
-      <c r="AA31" s="18">
+      <c r="E31" s="22"/>
+      <c r="F31" s="16">
         <v>61</v>
       </c>
-      <c r="AB31" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="AC31" s="19"/>
+      <c r="G31" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="H31" s="17"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="12"/>
+      <c r="T31" s="12"/>
+      <c r="U31" s="12"/>
+      <c r="V31" s="12"/>
+      <c r="W31" s="12"/>
+      <c r="X31" s="32"/>
+      <c r="Y31" s="32"/>
+      <c r="Z31" s="32"/>
+      <c r="AA31" s="12"/>
+      <c r="AB31" s="12"/>
+      <c r="AC31" s="12"/>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="2" t="s">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="19" t="s">
         <v>33</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="8"/>
-      <c r="U32" s="11"/>
-      <c r="V32" s="11"/>
-      <c r="W32" s="11"/>
-      <c r="X32" s="14"/>
-      <c r="Y32" s="14"/>
-      <c r="Z32" s="14"/>
-      <c r="AA32" s="18">
+      <c r="E32" s="22"/>
+      <c r="F32" s="16">
         <v>62</v>
       </c>
-      <c r="AB32" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="AC32" s="19"/>
+      <c r="G32" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="H32" s="17"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12"/>
+      <c r="S32" s="12"/>
+      <c r="T32" s="12"/>
+      <c r="U32" s="12"/>
+      <c r="V32" s="12"/>
+      <c r="W32" s="12"/>
+      <c r="X32" s="32"/>
+      <c r="Y32" s="32"/>
+      <c r="Z32" s="32"/>
+      <c r="AA32" s="12"/>
+      <c r="AB32" s="12"/>
+      <c r="AC32" s="12"/>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="2" t="s">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E33" s="3"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="11"/>
-      <c r="V33" s="11"/>
-      <c r="W33" s="11"/>
-      <c r="X33" s="14"/>
-      <c r="Y33" s="14"/>
-      <c r="Z33" s="14"/>
-      <c r="AA33" s="18">
+      <c r="E33" s="22"/>
+      <c r="F33" s="16">
         <v>63</v>
       </c>
-      <c r="AB33" s="18" t="s">
-        <v>262</v>
-      </c>
-      <c r="AC33" s="19"/>
+      <c r="G33" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="H33" s="17"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+      <c r="S33" s="12"/>
+      <c r="T33" s="12"/>
+      <c r="U33" s="12"/>
+      <c r="V33" s="12"/>
+      <c r="W33" s="12"/>
+      <c r="X33" s="32"/>
+      <c r="Y33" s="32"/>
+      <c r="Z33" s="32"/>
+      <c r="AA33" s="12"/>
+      <c r="AB33" s="12"/>
+      <c r="AC33" s="12"/>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="2" t="s">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="19" t="s">
         <v>35</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
-      <c r="S34" s="8"/>
-      <c r="T34" s="8"/>
-      <c r="U34" s="11"/>
-      <c r="V34" s="11"/>
-      <c r="W34" s="11"/>
-      <c r="X34" s="14"/>
-      <c r="Y34" s="14"/>
-      <c r="Z34" s="14"/>
-      <c r="AA34" s="18">
+      <c r="E34" s="22"/>
+      <c r="F34" s="16">
         <v>64</v>
       </c>
-      <c r="AB34" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="AC34" s="19"/>
+      <c r="G34" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="H34" s="17"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
+      <c r="S34" s="12"/>
+      <c r="T34" s="12"/>
+      <c r="U34" s="12"/>
+      <c r="V34" s="12"/>
+      <c r="W34" s="12"/>
+      <c r="X34" s="32"/>
+      <c r="Y34" s="32"/>
+      <c r="Z34" s="32"/>
+      <c r="AA34" s="12"/>
+      <c r="AB34" s="12"/>
+      <c r="AC34" s="12"/>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="2" t="s">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="19" t="s">
         <v>36</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-      <c r="T35" s="8"/>
-      <c r="U35" s="11"/>
-      <c r="V35" s="11"/>
-      <c r="W35" s="11"/>
-      <c r="X35" s="14"/>
-      <c r="Y35" s="14"/>
-      <c r="Z35" s="14"/>
-      <c r="AA35" s="18">
+      <c r="E35" s="22"/>
+      <c r="F35" s="16">
         <v>65</v>
       </c>
-      <c r="AB35" s="18" t="s">
-        <v>264</v>
-      </c>
-      <c r="AC35" s="19"/>
+      <c r="G35" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="H35" s="17"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="12"/>
+      <c r="P35" s="12"/>
+      <c r="Q35" s="12"/>
+      <c r="R35" s="12"/>
+      <c r="S35" s="12"/>
+      <c r="T35" s="12"/>
+      <c r="U35" s="12"/>
+      <c r="V35" s="12"/>
+      <c r="W35" s="12"/>
+      <c r="X35" s="32"/>
+      <c r="Y35" s="32"/>
+      <c r="Z35" s="32"/>
+      <c r="AA35" s="12"/>
+      <c r="AB35" s="12"/>
+      <c r="AC35" s="12"/>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="2" t="s">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="19" t="s">
         <v>37</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-      <c r="T36" s="8"/>
-      <c r="U36" s="11"/>
-      <c r="V36" s="11"/>
-      <c r="W36" s="11"/>
-      <c r="X36" s="14"/>
-      <c r="Y36" s="14"/>
-      <c r="Z36" s="14"/>
+      <c r="E36" s="22"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="12"/>
+      <c r="R36" s="12"/>
+      <c r="S36" s="12"/>
+      <c r="T36" s="12"/>
+      <c r="U36" s="32"/>
+      <c r="V36" s="32"/>
+      <c r="W36" s="32"/>
+      <c r="X36" s="12"/>
+      <c r="Y36" s="12"/>
+      <c r="Z36" s="12"/>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="2" t="s">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="19" t="s">
         <v>38</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="8"/>
-      <c r="T37" s="8"/>
-      <c r="U37" s="11"/>
-      <c r="V37" s="11"/>
-      <c r="W37" s="11"/>
-      <c r="X37" s="14"/>
-      <c r="Y37" s="14"/>
-      <c r="Z37" s="14"/>
+      <c r="E37" s="22"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
+      <c r="N37" s="12"/>
+      <c r="O37" s="12"/>
+      <c r="P37" s="12"/>
+      <c r="Q37" s="12"/>
+      <c r="R37" s="12"/>
+      <c r="S37" s="12"/>
+      <c r="T37" s="12"/>
+      <c r="U37" s="32"/>
+      <c r="V37" s="32"/>
+      <c r="W37" s="32"/>
+      <c r="X37" s="12"/>
+      <c r="Y37" s="12"/>
+      <c r="Z37" s="12"/>
     </row>
   </sheetData>
-  <dataValidations count="20">
+  <dataValidations count="19">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Enter an integer between 0 and 120" sqref="B4" xr:uid="{B1ED41BC-30F7-C54A-AE94-8016912BA55A}">
       <formula1>0</formula1>
       <formula2>120</formula2>
@@ -3586,58 +3658,55 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Please input either 'M' or 'F'" sqref="B5" xr:uid="{BC652F4B-BEAA-BE40-980A-D8D5DBBFFAAC}">
       <formula1>"M,F"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Enter either 'Y' or 'N'" sqref="H2:H29" xr:uid="{B18B96E8-2046-B24C-850F-5D4B23987964}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Enter either 'Y' or 'N'" sqref="K2:K29" xr:uid="{B18B96E8-2046-B24C-850F-5D4B23987964}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" sqref="Q16:Q17" xr:uid="{F40569F7-7A99-BB41-9B25-EBAC446CE1DB}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" sqref="T16:T17" xr:uid="{F40569F7-7A99-BB41-9B25-EBAC446CE1DB}">
       <formula1>0</formula1>
       <formula2>3</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Must be exactly 9 characters" sqref="B8" xr:uid="{315D64F4-676F-A44D-8C17-AD5ABE4B5005}">
-      <formula1>9</formula1>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Enter a number between 1 and 4" sqref="N2 N3 N4" xr:uid="{81B9F12B-CF19-7D4E-9CA0-65C5F88E251D}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Enter a number between 1 and 4" sqref="Q2 Q3 Q4" xr:uid="{81B9F12B-CF19-7D4E-9CA0-65C5F88E251D}">
       <formula1>1</formula1>
       <formula2>4</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Enter a number between 1 and 3" sqref="N6 N8:N9" xr:uid="{A6933A78-ED6E-B54F-8F9A-E167ACF76292}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Enter a number between 1 and 3" sqref="Q6 Q8:Q9" xr:uid="{A6933A78-ED6E-B54F-8F9A-E167ACF76292}">
       <formula1>1</formula1>
       <formula2>3</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input an integer between 0 and 4" sqref="Q2:Q15" xr:uid="{CEC098AE-182D-FA49-8CF0-EEB9E0847019}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input an integer between 0 and 4" sqref="T2:T15" xr:uid="{CEC098AE-182D-FA49-8CF0-EEB9E0847019}">
       <formula1>0</formula1>
       <formula2>4</formula2>
     </dataValidation>
-    <dataValidation operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Enter DOB in format DD.MM.YY" sqref="B9" xr:uid="{8677C5A0-DDA8-5744-BD30-25679193FB92}"/>
+    <dataValidation operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Enter DOB in format DD.MM.YY" sqref="B8" xr:uid="{8677C5A0-DDA8-5744-BD30-25679193FB92}"/>
     <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Max length 19 characters" sqref="B3" xr:uid="{F302C943-075C-5A46-BAE7-3AB0FDA9DACF}">
       <formula1>19</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" sqref="W6:W18" xr:uid="{26084A39-00B8-C041-BBAC-36E9A5281CFE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" sqref="Z6:Z18" xr:uid="{26084A39-00B8-C041-BBAC-36E9A5281CFE}">
       <formula1>"Y, N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Enter 2, 4, 6, 8" sqref="W2" xr:uid="{0BD65506-655B-F547-9827-C2B57BF4A76B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Enter 2, 4, 6, 8" sqref="Z2" xr:uid="{0BD65506-655B-F547-9827-C2B57BF4A76B}">
       <formula1>"2,4,6,8"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Enter an integer between 1 and 4" sqref="W3:W5" xr:uid="{BECF4D44-824A-F245-BE2B-EA7E9688BF84}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Enter an integer between 1 and 4" sqref="Z3:Z5" xr:uid="{BECF4D44-824A-F245-BE2B-EA7E9688BF84}">
       <formula1>1</formula1>
       <formula2>4</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input a number between 1 and 5" sqref="E2:E37 N7 N5" xr:uid="{271013E3-1423-A444-A8C6-4BCC80235AF0}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input a number between 1 and 5" sqref="E2:E37 Q7 Q5" xr:uid="{271013E3-1423-A444-A8C6-4BCC80235AF0}">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input a number between 0 and 3" sqref="K2:K17" xr:uid="{E7E4835E-9733-BC47-A84F-2F421F533EA4}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input a number between 0 and 3" sqref="N2:N17" xr:uid="{E7E4835E-9733-BC47-A84F-2F421F533EA4}">
       <formula1>0</formula1>
       <formula2>3</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input a number between 0 and 4" sqref="Z20:Z23 Z2:Z9 T2:T21" xr:uid="{F7AEEDA1-C641-A946-B2D6-50CF8F25AB41}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input a number between 0 and 4" sqref="AC20:AC23 AC2:AC9 W2:W21" xr:uid="{F7AEEDA1-C641-A946-B2D6-50CF8F25AB41}">
       <formula1>0</formula1>
       <formula2>4</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input either 'Y' or 'N'" sqref="Z10:Z19" xr:uid="{C45CB5A2-312A-9349-BC4A-AA78049DC6D5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input either 'Y' or 'N'" sqref="AC10:AC19" xr:uid="{C45CB5A2-312A-9349-BC4A-AA78049DC6D5}">
       <formula1>"Y, N"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input a number between 1 and 5." sqref="AC2:AC35" xr:uid="{C5C022E8-27A2-0343-A204-FA487880999E}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input a number between 1 and 5." sqref="H2:H35" xr:uid="{C5C022E8-27A2-0343-A204-FA487880999E}">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
slight changes to excel template
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksnelling/Desktop/form-creator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313A29A3-7B8C-A041-9373-0880DB3B6572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8BA7EC-B9AC-B643-8A11-95571B2C9EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18000" yWindow="880" windowWidth="18000" windowHeight="20600" xr2:uid="{5B803FEE-CBC5-CD4B-BFE8-7DF0DABD6B40}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20600" xr2:uid="{5B803FEE-CBC5-CD4B-BFE8-7DF0DABD6B40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2396,8 +2396,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="44" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4594,7 +4594,7 @@
       <c r="Z37" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="FmP5xU76/ALqoxSyUgngNpvUSgR5qza2I5Wup70oCw4o/1jKWMPLKtR7SSyc0yDXeBBtT7tdNqxCw0J23R4DuA==" saltValue="tZfiAQYmYrStbYkh4VDn/Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="19">
     <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Name must be less than 20 characters_x000a_" sqref="B5 B2" xr:uid="{91D9CADE-1361-894F-81E5-FC375AB75B27}">
       <formula1>19</formula1>

</xml_diff>

<commit_message>
minor change to excel template
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksnelling/Desktop/form-creator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8BA7EC-B9AC-B643-8A11-95571B2C9EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6530DCA7-C08F-C342-B3EC-8FF9B6BC6A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20600" xr2:uid="{5B803FEE-CBC5-CD4B-BFE8-7DF0DABD6B40}"/>
   </bookViews>
@@ -557,9 +557,6 @@
     <t>Nutrition</t>
   </si>
   <si>
-    <t>Other _desc</t>
-  </si>
-  <si>
     <t>1- not taking any listed meds
 2- taking one
 3- taking two
@@ -576,9 +573,6 @@
 2- AMTS 7 or 8 OR mildly impaired
 3- AMTS 5 or 6 OR moderately impaired
 4- AMTS 4 or less OR severely impaired</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if select 'Y' enter details below </t>
   </si>
   <si>
     <t>2- none in last 12 months
@@ -1470,19 +1464,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Other </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>(mark yes or no)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Sexual</t>
     </r>
     <r>
@@ -1788,6 +1769,44 @@
   </si>
   <si>
     <t xml:space="preserve">If you wish to add a comment for Question 8, enter here -&gt; </t>
+  </si>
+  <si>
+    <t>Other_desc</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>Are there any other risk factors?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+if select 'Y' enter details below </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Other </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>(mark yes or no)
+If Yes enter details below</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1975,7 +1994,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2052,6 +2071,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2396,8 +2418,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="44" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="P9" zoomScale="75" workbookViewId="0">
+      <selection activeCell="Z19" sqref="Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2432,7 +2454,7 @@
     <col min="28" max="28" width="66.5" style="8" customWidth="1"/>
     <col min="29" max="29" width="21.33203125" style="8" customWidth="1"/>
     <col min="30" max="30" width="10.6640625"/>
-    <col min="31" max="31" width="51.83203125" customWidth="1"/>
+    <col min="31" max="31" width="63" customWidth="1"/>
     <col min="32" max="32" width="20.5" customWidth="1"/>
     <col min="33" max="16384" width="10.83203125" style="8"/>
   </cols>
@@ -2448,25 +2470,25 @@
         <v>37</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>38</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J1" s="17" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="K1" s="17" t="s">
         <v>39</v>
@@ -2475,7 +2497,7 @@
         <v>101</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="N1" s="17" t="s">
         <v>102</v>
@@ -2502,7 +2524,7 @@
         <v>133</v>
       </c>
       <c r="V1" s="17" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="W1" s="17" t="s">
         <v>134</v>
@@ -2517,22 +2539,22 @@
         <v>158</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="AB1" s="17" t="s">
         <v>44</v>
       </c>
       <c r="AC1" s="19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="AD1" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="AE1" s="18" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="AF1" s="18" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="119" x14ac:dyDescent="0.2">
@@ -2551,7 +2573,7 @@
         <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="3">
@@ -2572,14 +2594,14 @@
         <v>121</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="3">
         <v>1</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="3">
@@ -2593,21 +2615,21 @@
         <v>159</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="3">
         <v>1</v>
       </c>
       <c r="AB2" s="16" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AC2" s="12"/>
       <c r="AD2" s="3">
         <v>1</v>
       </c>
       <c r="AE2" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="AF2" s="2"/>
     </row>
@@ -2627,7 +2649,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="3">
@@ -2648,14 +2670,14 @@
         <v>122</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="3">
         <v>2</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="3">
@@ -2669,21 +2691,21 @@
         <v>160</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Z3" s="2"/>
       <c r="AA3" s="3">
         <v>2</v>
       </c>
       <c r="AB3" s="16" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="AC3" s="12"/>
       <c r="AD3" s="3">
         <v>2</v>
       </c>
       <c r="AE3" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="AF3" s="2"/>
     </row>
@@ -2703,7 +2725,7 @@
         <v>13</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="3">
@@ -2724,14 +2746,14 @@
         <v>123</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" s="3">
         <v>3</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="T4" s="2"/>
       <c r="U4" s="3">
@@ -2745,21 +2767,21 @@
         <v>161</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Z4" s="2"/>
       <c r="AA4" s="3">
         <v>3</v>
       </c>
       <c r="AB4" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="AC4" s="12"/>
       <c r="AD4" s="3">
         <v>3</v>
       </c>
       <c r="AE4" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="AF4" s="2"/>
     </row>
@@ -2779,7 +2801,7 @@
         <v>14</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="3">
@@ -2800,14 +2822,14 @@
         <v>124</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="3">
         <v>4</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="T5" s="2"/>
       <c r="U5" s="3">
@@ -2821,21 +2843,21 @@
         <v>162</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Z5" s="2"/>
       <c r="AA5" s="3">
         <v>4</v>
       </c>
       <c r="AB5" s="16" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="AC5" s="12"/>
       <c r="AD5" s="3">
         <v>4</v>
       </c>
       <c r="AE5" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="AF5" s="2"/>
     </row>
@@ -2855,7 +2877,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="3">
@@ -2876,14 +2898,14 @@
         <v>125</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="Q6" s="2"/>
       <c r="R6" s="3">
         <v>5</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T6" s="2"/>
       <c r="U6" s="3">
@@ -2897,27 +2919,27 @@
         <v>163</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="Z6" s="2"/>
       <c r="AA6" s="3">
         <v>5</v>
       </c>
       <c r="AB6" s="16" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="AC6" s="12"/>
       <c r="AD6" s="3">
         <v>5</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="AF6" s="2"/>
     </row>
     <row r="7" spans="1:36" ht="119" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="1" t="s">
@@ -2931,7 +2953,7 @@
         <v>16</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="3">
@@ -2952,14 +2974,14 @@
         <v>126</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="3">
         <v>6</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="T7" s="2"/>
       <c r="U7" s="3">
@@ -2973,25 +2995,25 @@
         <v>164</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="Z7" s="2"/>
       <c r="AA7" s="3">
         <v>6</v>
       </c>
       <c r="AB7" s="16" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="AC7" s="12"/>
       <c r="AD7" s="3">
         <v>6</v>
       </c>
       <c r="AE7" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="AF7" s="2"/>
       <c r="AJ7" s="8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:36" ht="102" x14ac:dyDescent="0.2">
@@ -3006,7 +3028,7 @@
         <v>21</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="3">
@@ -3027,14 +3049,14 @@
         <v>127</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="3">
         <v>7</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="T8" s="2"/>
       <c r="U8" s="3">
@@ -3048,21 +3070,21 @@
         <v>165</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="Z8" s="2"/>
       <c r="AA8" s="3">
         <v>7</v>
       </c>
       <c r="AB8" s="16" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="AC8" s="12"/>
       <c r="AD8" s="3">
         <v>7</v>
       </c>
       <c r="AE8" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="AF8" s="2"/>
     </row>
@@ -3078,7 +3100,7 @@
         <v>22</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="3">
@@ -3099,14 +3121,14 @@
         <v>128</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="3">
         <v>8</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="T9" s="2"/>
       <c r="U9" s="3">
@@ -3120,21 +3142,21 @@
         <v>166</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="Z9" s="2"/>
       <c r="AA9" s="3">
         <v>8</v>
       </c>
       <c r="AB9" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AC9" s="12"/>
       <c r="AD9" s="3">
         <v>8</v>
       </c>
       <c r="AE9" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="AF9" s="2"/>
     </row>
@@ -3152,7 +3174,7 @@
         <v>23</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="3">
@@ -3176,7 +3198,7 @@
         <v>9</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="T10" s="2"/>
       <c r="U10" s="3">
@@ -3190,21 +3212,21 @@
         <v>131</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="Z10" s="2"/>
       <c r="AA10" s="3" t="s">
         <v>121</v>
       </c>
       <c r="AB10" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC10" s="12"/>
       <c r="AD10" s="3">
         <v>9</v>
       </c>
       <c r="AE10" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="AF10" s="2"/>
     </row>
@@ -3222,7 +3244,7 @@
         <v>24</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="3">
@@ -3246,7 +3268,7 @@
         <v>10</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="T11" s="2"/>
       <c r="U11" s="3">
@@ -3260,21 +3282,21 @@
         <v>167</v>
       </c>
       <c r="Y11" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="Z11" s="2"/>
       <c r="AA11" s="3" t="s">
         <v>122</v>
       </c>
       <c r="AB11" s="3" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="AC11" s="12"/>
       <c r="AD11" s="3">
         <v>10</v>
       </c>
       <c r="AE11" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="AF11" s="2"/>
     </row>
@@ -3292,7 +3314,7 @@
         <v>25</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="3">
@@ -3316,7 +3338,7 @@
         <v>11</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="T12" s="2"/>
       <c r="U12" s="3">
@@ -3330,21 +3352,21 @@
         <v>168</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="Z12" s="2"/>
       <c r="AA12" s="3" t="s">
         <v>123</v>
       </c>
       <c r="AB12" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="AC12" s="12"/>
       <c r="AD12" s="3">
         <v>11</v>
       </c>
       <c r="AE12" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="AF12" s="2"/>
     </row>
@@ -3362,7 +3384,7 @@
         <v>31</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="3">
@@ -3386,7 +3408,7 @@
         <v>12</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="T13" s="2"/>
       <c r="U13" s="3">
@@ -3400,21 +3422,21 @@
         <v>169</v>
       </c>
       <c r="Y13" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="Z13" s="2"/>
       <c r="AA13" s="3" t="s">
         <v>124</v>
       </c>
       <c r="AB13" s="3" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="AC13" s="12"/>
       <c r="AD13" s="3">
         <v>12</v>
       </c>
       <c r="AE13" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="AF13" s="2"/>
     </row>
@@ -3432,7 +3454,7 @@
         <v>32</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="3">
@@ -3456,7 +3478,7 @@
         <v>13</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="T14" s="2"/>
       <c r="U14" s="3">
@@ -3470,21 +3492,21 @@
         <v>170</v>
       </c>
       <c r="Y14" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="Z14" s="2"/>
       <c r="AA14" s="3" t="s">
         <v>125</v>
       </c>
       <c r="AB14" s="3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="AC14" s="12"/>
       <c r="AD14" s="3">
         <v>13</v>
       </c>
       <c r="AE14" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="AF14" s="2"/>
     </row>
@@ -3502,7 +3524,7 @@
         <v>33</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="3">
@@ -3526,7 +3548,7 @@
         <v>14</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="T15" s="2"/>
       <c r="U15" s="3">
@@ -3540,21 +3562,21 @@
         <v>171</v>
       </c>
       <c r="Y15" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="Z15" s="2"/>
       <c r="AA15" s="3" t="s">
         <v>126</v>
       </c>
       <c r="AB15" s="3" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="AC15" s="12"/>
       <c r="AD15" s="3">
         <v>14</v>
       </c>
       <c r="AE15" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="AF15" s="2"/>
     </row>
@@ -3572,7 +3594,7 @@
         <v>34</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="3">
@@ -3606,21 +3628,21 @@
         <v>172</v>
       </c>
       <c r="Y16" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="Z16" s="2"/>
       <c r="AA16" s="3" t="s">
         <v>127</v>
       </c>
       <c r="AB16" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="AC16" s="12"/>
       <c r="AD16" s="3">
         <v>15</v>
       </c>
       <c r="AE16" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="AF16" s="2"/>
     </row>
@@ -3638,7 +3660,7 @@
         <v>41</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="3">
@@ -3672,21 +3694,21 @@
         <v>82</v>
       </c>
       <c r="Y17" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Z17" s="2"/>
       <c r="AA17" s="3" t="s">
         <v>128</v>
       </c>
       <c r="AB17" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="AC17" s="12"/>
       <c r="AD17" s="3">
         <v>16</v>
       </c>
       <c r="AE17" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="AF17" s="2"/>
     </row>
@@ -3704,7 +3726,7 @@
         <v>42</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="3">
@@ -3733,22 +3755,22 @@
       <c r="X18" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="Y18" s="7" t="s">
-        <v>177</v>
+      <c r="Y18" s="24" t="s">
+        <v>318</v>
       </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="AB18" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="AC18" s="12"/>
       <c r="AD18" s="3">
         <v>17</v>
       </c>
       <c r="AE18" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="AF18" s="2"/>
     </row>
@@ -3766,7 +3788,7 @@
         <v>43</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="3">
@@ -3793,28 +3815,28 @@
       </c>
       <c r="W19" s="2"/>
       <c r="X19" s="3" t="s">
-        <v>173</v>
+        <v>317</v>
       </c>
       <c r="Y19" s="7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="Z19" s="2"/>
       <c r="AA19" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="AB19" s="4" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="AC19" s="12"/>
       <c r="AD19" s="3">
         <v>18</v>
       </c>
       <c r="AE19" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="AF19" s="2"/>
     </row>
-    <row r="20" spans="1:32" ht="102" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="1" t="s">
@@ -3857,18 +3879,18 @@
       <c r="X20" s="14"/>
       <c r="Y20" s="14"/>
       <c r="Z20" s="14"/>
-      <c r="AA20" s="3">
-        <v>9</v>
-      </c>
-      <c r="AB20" s="16" t="s">
-        <v>308</v>
-      </c>
-      <c r="AC20" s="12"/>
+      <c r="AA20" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="AB20" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="AC20" s="2"/>
       <c r="AD20" s="3">
         <v>19</v>
       </c>
       <c r="AE20" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="AF20" s="2"/>
     </row>
@@ -3886,7 +3908,7 @@
         <v>45</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="3">
@@ -3916,17 +3938,17 @@
       <c r="Y21" s="14"/>
       <c r="Z21" s="14"/>
       <c r="AA21" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AB21" s="16" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="AC21" s="12"/>
       <c r="AD21" s="3">
         <v>20</v>
       </c>
       <c r="AE21" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AF21" s="2"/>
     </row>
@@ -3944,7 +3966,7 @@
         <v>51</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="3">
@@ -3970,14 +3992,14 @@
       <c r="Y22" s="14"/>
       <c r="Z22" s="14"/>
       <c r="AA22" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AB22" s="16" t="s">
-        <v>310</v>
-      </c>
-      <c r="AC22" s="2"/>
+        <v>306</v>
+      </c>
+      <c r="AC22" s="12"/>
     </row>
-    <row r="23" spans="1:32" ht="119" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" ht="102" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="1" t="s">
@@ -3991,7 +4013,7 @@
         <v>52</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="3">
@@ -4017,14 +4039,14 @@
       <c r="Y23" s="14"/>
       <c r="Z23" s="14"/>
       <c r="AA23" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB23" s="16" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="AC23" s="2"/>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" ht="119" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="1" t="s">
@@ -4038,7 +4060,7 @@
         <v>53</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H24" s="22"/>
       <c r="I24" s="3">
@@ -4063,11 +4085,11 @@
       <c r="X24" s="14"/>
       <c r="Y24" s="14"/>
       <c r="Z24" s="14"/>
-      <c r="AA24" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="AB24" s="15" t="s">
-        <v>319</v>
+      <c r="AA24" s="3">
+        <v>12</v>
+      </c>
+      <c r="AB24" s="16" t="s">
+        <v>308</v>
       </c>
       <c r="AC24" s="2"/>
     </row>
@@ -4085,7 +4107,7 @@
         <v>54</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H25" s="22"/>
       <c r="I25" s="3">
@@ -4120,14 +4142,14 @@
         <v>25</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="10">
         <v>55</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H26" s="22"/>
       <c r="I26" s="3">
@@ -4163,14 +4185,14 @@
         <v>26</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="10">
         <v>56</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H27" s="22"/>
       <c r="I27" s="3">
@@ -4195,9 +4217,6 @@
       <c r="X27" s="14"/>
       <c r="Y27" s="14"/>
       <c r="Z27" s="14"/>
-      <c r="AA27" s="9"/>
-      <c r="AB27" s="9"/>
-      <c r="AC27" s="9"/>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
@@ -4206,14 +4225,14 @@
         <v>27</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="10">
         <v>57</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H28" s="22"/>
       <c r="I28" s="3">
@@ -4249,14 +4268,14 @@
         <v>28</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="10">
         <v>58</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H29" s="22"/>
       <c r="I29" s="11">
@@ -4292,21 +4311,21 @@
         <v>29</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="10">
         <v>59</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="K30" s="2"/>
       <c r="L30" s="9"/>
@@ -4342,14 +4361,14 @@
         <v>61</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H31" s="22"/>
       <c r="I31" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J31" s="15" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="9"/>
@@ -4385,14 +4404,14 @@
         <v>62</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H32" s="22"/>
       <c r="I32" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="9"/>
@@ -4428,14 +4447,14 @@
         <v>63</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H33" s="22"/>
       <c r="I33" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J33" s="15" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="9"/>
@@ -4471,7 +4490,7 @@
         <v>64</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H34" s="22"/>
       <c r="I34" s="9"/>
@@ -4510,7 +4529,7 @@
         <v>65</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H35" s="22"/>
       <c r="I35" s="9"/>
@@ -4594,7 +4613,7 @@
       <c r="Z37" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="FmP5xU76/ALqoxSyUgngNpvUSgR5qza2I5Wup70oCw4o/1jKWMPLKtR7SSyc0yDXeBBtT7tdNqxCw0J23R4DuA==" saltValue="tZfiAQYmYrStbYkh4VDn/Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="3c/CXzDDfCRUyF3fzx4RtSIBf0joJnlL3fr1RID1IdYqS5khqTT5opjmcfzkY8ZBnnJiKhfEeyt4trvRzc0RkA==" saltValue="lahht0po8xXHl5HNEmq0eg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="19">
     <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Name must be less than 20 characters_x000a_" sqref="B5 B2" xr:uid="{91D9CADE-1361-894F-81E5-FC375AB75B27}">
       <formula1>19</formula1>
@@ -4643,7 +4662,7 @@
       <formula1>0</formula1>
       <formula2>3</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input a number between 0 and 4" sqref="AC20:AC23 AC2:AC9 W2:W21 AF2:AF21" xr:uid="{F7AEEDA1-C641-A946-B2D6-50CF8F25AB41}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input a number between 0 and 4" sqref="AC21:AC24 AC2:AC9 W2:W21 AF2:AF21" xr:uid="{F7AEEDA1-C641-A946-B2D6-50CF8F25AB41}">
       <formula1>0</formula1>
       <formula2>4</formula2>
     </dataValidation>
@@ -4657,7 +4676,7 @@
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" sqref="K30:K33" xr:uid="{7CC4C9CF-B45E-3D4B-9044-97043DD3C98F}">
       <formula1>40</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Message must be less than 40 characters" sqref="AC24" xr:uid="{D33F11B3-65C5-1F4F-93EC-CA5ED38EB5A9}">
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Message must be less than 40 characters" sqref="AC20" xr:uid="{D33F11B3-65C5-1F4F-93EC-CA5ED38EB5A9}">
       <formula1>40</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added HONOSCA form to application.
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksnelling/Desktop/form-creator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF10157-D181-6C44-AACF-00450A370D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE1FC0F-39AC-434E-A712-C4B44C3F67A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13440" yWindow="900" windowWidth="22560" windowHeight="20600" xr2:uid="{5B803FEE-CBC5-CD4B-BFE8-7DF0DABD6B40}"/>
+    <workbookView xWindow="2880" yWindow="900" windowWidth="33120" windowHeight="20600" xr2:uid="{5B803FEE-CBC5-CD4B-BFE8-7DF0DABD6B40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="333">
   <si>
     <t>gender</t>
   </si>
@@ -6673,31 +6673,6 @@
         <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Problems associated with hallucination and delusions
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>0 = no evidence of hallucination or delusons
-1 = somewhat odd or eccentric beliefs
-2 = delusions or hallucinations are presents but little distress to patient
-3 = marked preoccupation with delusions or hallucinations, causing much distress
-4 = mental state is seriously affected by delusions or hallucinations</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">Problems with depressed mood
 </t>
     </r>
@@ -7123,6 +7098,414 @@
 2 = very limited
 1 = unable
 0 = N/A</t>
+    </r>
+  </si>
+  <si>
+    <t>HONOSCA</t>
+  </si>
+  <si>
+    <t>HONOSCA Values</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Problems with disruptive, antisocial or aggressive behaviour</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0 = no problems
+1 = minor quarrelling, demanding behaviour, undue irritability, lying etc.
+2 = mild disruptive or antisocial behaviour, lesser damage to property, or aggression, or defiance
+3 = moderately severe aggressive or antisocial behaviour such as fighting or persistently threatening or very oppositional or more serious destruction to property or moderate delinquent acts.
+4 = disruptive in almost all activities, or at least one serious physical attack on others or animals, or serious destruction to property.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problems with overactivity, attention or concentration
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0 = no problems
+1 = slight overactivity or minor restlessness
+2 = mild but definite overactivity and/or attentional problems but these can usually be controlled.
+3 = moderately severe overactivity and/or attentional problems that are sometimes uncontrollable.
+4 = severe overactivity or attentional problems that are present in most activities and not controllable.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Non-accidental self-injury
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0 = no problems
+1 = occasional thoughs about death, or of self harm not leading to injury.
+2 = non-hazardous self harm, such as wrist scratching, whether or not associated with suicidal thoughts
+3 = moderately severe suicidal intent or moderate non hazardous self harm
+4 = serious sucidual attempt and/or serious deliberate self-harm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Problems with alcohol, substance/solvent misuse
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0 = no problems
+1 = minor alcohol or drug use, within age norms
+2 = mildly excessive alcohol or drug use
+3 = moderately severe drug or alcohol problems significantly out of keeping with age norms
+4 = severe drug or alcohol problems leading to dependency or incapacity</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Problems with scholastic or language skills
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0 = no problems
+1 = minor impairment within the normal range of variation
+2 = mild but definite impairment of clinical significance
+3 = moderately severe problem, below level expected on the basis of mental age, past performance or disability
+4 = severe impairment much below  level expected on the basis of mental age, past performance or disability</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Physical illness or disability problems
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0 = no problems
+1 = slight incapacity as a result of a health problem
+2 = physical health roblem imposes mild but definite functional restriction
+3 = moderate degree of restriction on activity due to physical health problem
+4 = severe or complete incapacity due to physical health problem</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Problems associated with hallucination and delusions
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0 = no evidence of hallucination or delusons
+1 = somewhat odd or eccentric beliefs
+2 = delusions or hallucinations are present but little distress to patient
+3 = marked preoccupation with delusions or hallucinations, causing much distress
+4 = mental state is seriously affected by delusions or hallucinations</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Problems associated with hallucination, delusions or abnormal perceptions
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0 = no evidence ofabnormal thoughts or perceptions
+1 = somewhat odd or eccentric beliefs
+2 = abnormal thoughts or perceptions are present but little distress to patient
+3 = moderate preoccupation with abnormal thoughts,  perceptions,  delusions or hallucinations, causing distress
+4 = mental state and behaviour is seriously affected by delusions or hallucinations</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t xml:space="preserve">Problems with non organic somatic symptoms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0 = no problems
+1 = slight problems only like occasional enuresis, minor sleep problems, headaches or stomach-aches
+2 = mild but definite problem with non organic somatic symptoms
+3 = moderately severe, symptoms produce a moderate degree of restriciton in some activities
+4 = very severe or symptoms persist into most activities</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Problems with emotional and related sympyoms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0 = no problems
+1 = mildly anxious; gloomy; or transient mood changes
+2 = mild but definite emotional sympotoms is clinically present but is not preoccupying
+3 = moderately severe emotional symptoms, preoccupying, intruding activities and uncontrollable sometimes
+4 = severe emotional symptoms introducing into all activities, nearly always uncontrollable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Problems with peer relationships
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0 = no significant problems during the period
+1 = either transient or slight problems, occasional social withdrawal
+2 = mild but definite problems in making or sustaining peer relationships
+3 = pmoderate problems due to active or passive withdrawal from social relationships
+4 = severe social isolation due to inability to communicate socially or withdrawal</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Problems with self care and independence
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0 = no problems
+1 = minor problems only
+2 = self-care adequate, but definite inability to perform one or more complex skills
+3 = major problems in one or more areas of self-care or inability to perform several complex skills
+4 = severe disability or incapacity in all areas of self-care and complex skills</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Problems with family life and relationships
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0 = no problems
+1 = slight or transient problems
+2 = mild but definite problem
+3 = moderate problem. Problems associated with family/carer breakdown or reorganisation
+4 = serious problems with child feeling or being victimised, abused or seriously neglected by family or carer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Poor school attendance
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0 = no problems
+1 = slight problems; e.g., late for 2+ lessons
+2 = definite but mild problems, e.g., missed severel lessons or refusal to attend school
+3 = marked problems, absent severeal days during the period rated
+4 = severe problems, absent most or all days</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Problems with knowledge or undertsanding about the nature of the child's difficulties (last 2 weeks)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0 = no problems
+1 = slight problems
+2 = mild but definite problem
+3 = moderately severe problems. Parents have very little or incorrect knowledge about the problem
+4 = Very severe problem. Parents have no understanding about the nature of their child's problems</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Problems with lack of information about services or management of the child's difficulties
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0 = no problems
+1 = slight problems
+2 = mild but definite problem
+3 = moderately severe problems. Parents have  little information about appropriate services or professionals
+4 = Very severe problem. Parents have no information about appropriate services or professionals</t>
     </r>
   </si>
 </sst>
@@ -7133,7 +7516,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7332,7 +7715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7421,6 +7804,22 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7765,16 +8164,16 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="86" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="25" workbookViewId="0">
+      <selection activeCell="AF9" sqref="AF9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="29.1640625" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="63.6640625" customWidth="1"/>
+    <col min="4" max="4" width="73.6640625" customWidth="1"/>
     <col min="5" max="5" width="27.1640625" customWidth="1"/>
     <col min="6" max="6" width="22.5" style="6" customWidth="1"/>
     <col min="7" max="7" width="90.33203125" style="6" customWidth="1"/>
@@ -7789,7 +8188,7 @@
     <col min="16" max="16" width="80.33203125" customWidth="1"/>
     <col min="17" max="17" width="24.6640625" customWidth="1"/>
     <col min="18" max="18" width="10.6640625"/>
-    <col min="19" max="19" width="74.83203125" customWidth="1"/>
+    <col min="19" max="19" width="92.1640625" customWidth="1"/>
     <col min="20" max="20" width="21.33203125" customWidth="1"/>
     <col min="21" max="21" width="16.83203125" customWidth="1"/>
     <col min="22" max="22" width="59.1640625" customWidth="1"/>
@@ -7798,15 +8197,18 @@
     <col min="25" max="25" width="62.1640625" style="6" customWidth="1"/>
     <col min="26" max="26" width="18.5" style="6" customWidth="1"/>
     <col min="27" max="27" width="14.6640625" style="6" customWidth="1"/>
-    <col min="28" max="28" width="86" style="6" customWidth="1"/>
+    <col min="28" max="28" width="106" style="6" customWidth="1"/>
     <col min="29" max="29" width="21.33203125" style="6" customWidth="1"/>
-    <col min="30" max="30" width="10.6640625"/>
-    <col min="31" max="31" width="98.5" customWidth="1"/>
-    <col min="32" max="32" width="20.5" customWidth="1"/>
-    <col min="33" max="16384" width="10.83203125" style="6"/>
+    <col min="30" max="30" width="17.33203125" customWidth="1"/>
+    <col min="31" max="31" width="127.33203125" customWidth="1"/>
+    <col min="32" max="32" width="25.1640625" customWidth="1"/>
+    <col min="33" max="33" width="10.83203125" style="6"/>
+    <col min="34" max="34" width="130.33203125" style="6" customWidth="1"/>
+    <col min="35" max="35" width="25.83203125" style="6" customWidth="1"/>
+    <col min="36" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" ht="24">
       <c r="A1" s="13" t="s">
         <v>40</v>
       </c>
@@ -7894,17 +8296,26 @@
       <c r="AC1" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="AD1" s="14" t="s">
+      <c r="AD1" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="AE1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF1" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="AG1" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="AE1" s="14" t="s">
+      <c r="AH1" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="AF1" s="14" t="s">
+      <c r="AI1" s="14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="140" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" ht="173" customHeight="1">
       <c r="A2" s="27" t="s">
         <v>65</v>
       </c>
@@ -7975,12 +8386,19 @@
       <c r="AD2" s="3">
         <v>1</v>
       </c>
-      <c r="AE2" s="20" t="s">
+      <c r="AE2" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="AF2" s="2"/>
+      <c r="AI2" s="2"/>
     </row>
-    <row r="3" spans="1:36" ht="140" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" ht="132" customHeight="1">
       <c r="A3" s="27" t="s">
         <v>66</v>
       </c>
@@ -8051,12 +8469,19 @@
       <c r="AD3" s="3">
         <v>2</v>
       </c>
-      <c r="AE3" s="20" t="s">
+      <c r="AE3" s="31" t="s">
+        <v>318</v>
+      </c>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="3">
+        <v>2</v>
+      </c>
+      <c r="AH3" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="AF3" s="2"/>
+      <c r="AI3" s="2"/>
     </row>
-    <row r="4" spans="1:36" ht="140" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" ht="140">
       <c r="A4" s="27" t="s">
         <v>0</v>
       </c>
@@ -8127,12 +8552,19 @@
       <c r="AD4" s="3">
         <v>3</v>
       </c>
-      <c r="AE4" s="20" t="s">
+      <c r="AE4" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="AF4" s="10"/>
+      <c r="AG4" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH4" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="AF4" s="2"/>
+      <c r="AI4" s="2"/>
     </row>
-    <row r="5" spans="1:36" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" ht="136" customHeight="1">
       <c r="A5" s="27" t="s">
         <v>42</v>
       </c>
@@ -8203,12 +8635,19 @@
       <c r="AD5" s="3">
         <v>4</v>
       </c>
-      <c r="AE5" s="20" t="s">
+      <c r="AE5" s="26" t="s">
+        <v>320</v>
+      </c>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="3">
+        <v>4</v>
+      </c>
+      <c r="AH5" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="AF5" s="2"/>
+      <c r="AI5" s="2"/>
     </row>
-    <row r="6" spans="1:36" ht="120" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" ht="129" customHeight="1">
       <c r="A6" s="27" t="s">
         <v>62</v>
       </c>
@@ -8279,12 +8718,19 @@
       <c r="AD6" s="3">
         <v>5</v>
       </c>
-      <c r="AE6" s="20" t="s">
+      <c r="AE6" s="26" t="s">
+        <v>321</v>
+      </c>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="3">
+        <v>5</v>
+      </c>
+      <c r="AH6" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="AF6" s="2"/>
+      <c r="AI6" s="2"/>
     </row>
-    <row r="7" spans="1:36" ht="120" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" ht="149" customHeight="1">
       <c r="A7" s="27" t="s">
         <v>99</v>
       </c>
@@ -8349,21 +8795,28 @@
         <v>6</v>
       </c>
       <c r="AB7" s="26" t="s">
-        <v>298</v>
+        <v>323</v>
       </c>
       <c r="AC7" s="10"/>
       <c r="AD7" s="3">
         <v>6</v>
       </c>
-      <c r="AE7" s="20" t="s">
+      <c r="AE7" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="3">
+        <v>6</v>
+      </c>
+      <c r="AH7" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="AF7" s="2"/>
+      <c r="AI7" s="2"/>
       <c r="AJ7" s="6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="140" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" ht="160" customHeight="1">
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
@@ -8424,18 +8877,25 @@
         <v>7</v>
       </c>
       <c r="AB8" s="26" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AC8" s="10"/>
       <c r="AD8" s="3">
         <v>7</v>
       </c>
-      <c r="AE8" s="20" t="s">
+      <c r="AE8" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="3">
+        <v>7</v>
+      </c>
+      <c r="AH8" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="AF8" s="2"/>
+      <c r="AI8" s="2"/>
     </row>
-    <row r="9" spans="1:36" ht="140" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" ht="164" customHeight="1">
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
@@ -8496,18 +8956,25 @@
         <v>8</v>
       </c>
       <c r="AB9" s="20" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AC9" s="10"/>
       <c r="AD9" s="3">
         <v>8</v>
       </c>
-      <c r="AE9" s="20" t="s">
+      <c r="AE9" s="25" t="s">
+        <v>325</v>
+      </c>
+      <c r="AF9" s="32"/>
+      <c r="AG9" s="3">
+        <v>8</v>
+      </c>
+      <c r="AH9" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="AF9" s="2"/>
+      <c r="AI9" s="2"/>
     </row>
-    <row r="10" spans="1:36" ht="120" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" ht="145" customHeight="1">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="1" t="s">
@@ -8566,18 +9033,25 @@
         <v>51</v>
       </c>
       <c r="AB10" s="20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AC10" s="10"/>
       <c r="AD10" s="3">
         <v>9</v>
       </c>
-      <c r="AE10" s="20" t="s">
+      <c r="AE10" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="AF10" s="10"/>
+      <c r="AG10" s="3">
+        <v>9</v>
+      </c>
+      <c r="AH10" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="AF10" s="2"/>
+      <c r="AI10" s="2"/>
     </row>
-    <row r="11" spans="1:36" ht="120" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" ht="137" customHeight="1">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="1" t="s">
@@ -8636,18 +9110,25 @@
         <v>52</v>
       </c>
       <c r="AB11" s="20" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AC11" s="10"/>
       <c r="AD11" s="3">
         <v>10</v>
       </c>
-      <c r="AE11" s="20" t="s">
+      <c r="AE11" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF11" s="10"/>
+      <c r="AG11" s="3">
+        <v>10</v>
+      </c>
+      <c r="AH11" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="AF11" s="2"/>
+      <c r="AI11" s="2"/>
     </row>
-    <row r="12" spans="1:36" ht="120" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" ht="140" customHeight="1">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="1" t="s">
@@ -8706,18 +9187,25 @@
         <v>53</v>
       </c>
       <c r="AB12" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AC12" s="10"/>
       <c r="AD12" s="3">
         <v>11</v>
       </c>
-      <c r="AE12" s="20" t="s">
+      <c r="AE12" s="26" t="s">
+        <v>328</v>
+      </c>
+      <c r="AF12" s="10"/>
+      <c r="AG12" s="3">
+        <v>11</v>
+      </c>
+      <c r="AH12" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="AF12" s="2"/>
+      <c r="AI12" s="2"/>
     </row>
-    <row r="13" spans="1:36" ht="141" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" ht="156" customHeight="1">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="1" t="s">
@@ -8776,18 +9264,25 @@
         <v>54</v>
       </c>
       <c r="AB13" s="20" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AC13" s="10"/>
       <c r="AD13" s="3">
         <v>12</v>
       </c>
-      <c r="AE13" s="20" t="s">
+      <c r="AE13" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="3">
+        <v>12</v>
+      </c>
+      <c r="AH13" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="AF13" s="2"/>
+      <c r="AI13" s="2"/>
     </row>
-    <row r="14" spans="1:36" ht="143" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" ht="152" customHeight="1">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="1" t="s">
@@ -8846,18 +9341,25 @@
         <v>55</v>
       </c>
       <c r="AB14" s="20" t="s">
-        <v>305</v>
-      </c>
-      <c r="AC14" s="10"/>
+        <v>304</v>
+      </c>
+      <c r="AC14" s="2"/>
       <c r="AD14" s="3">
         <v>13</v>
       </c>
-      <c r="AE14" s="20" t="s">
+      <c r="AE14" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="3">
+        <v>13</v>
+      </c>
+      <c r="AH14" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="AF14" s="2"/>
+      <c r="AI14" s="2"/>
     </row>
-    <row r="15" spans="1:36" ht="140" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" ht="144" customHeight="1">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="1" t="s">
@@ -8916,18 +9418,25 @@
         <v>56</v>
       </c>
       <c r="AB15" s="20" t="s">
-        <v>304</v>
-      </c>
-      <c r="AC15" s="10"/>
+        <v>303</v>
+      </c>
+      <c r="AC15" s="2"/>
       <c r="AD15" s="3">
         <v>14</v>
       </c>
-      <c r="AE15" s="20" t="s">
+      <c r="AE15" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="AF15" s="2"/>
+      <c r="AG15" s="3">
+        <v>14</v>
+      </c>
+      <c r="AH15" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="AF15" s="2"/>
+      <c r="AI15" s="2"/>
     </row>
-    <row r="16" spans="1:36" ht="140" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" ht="156" customHeight="1">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="1" t="s">
@@ -8982,18 +9491,25 @@
         <v>57</v>
       </c>
       <c r="AB16" s="20" t="s">
-        <v>303</v>
-      </c>
-      <c r="AC16" s="10"/>
+        <v>302</v>
+      </c>
+      <c r="AC16" s="2"/>
       <c r="AD16" s="3">
         <v>15</v>
       </c>
-      <c r="AE16" s="20" t="s">
+      <c r="AE16" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="3">
+        <v>15</v>
+      </c>
+      <c r="AH16" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="AF16" s="2"/>
+      <c r="AI16" s="2"/>
     </row>
-    <row r="17" spans="1:32" ht="120" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:35" ht="134" customHeight="1">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="1" t="s">
@@ -9048,18 +9564,21 @@
         <v>58</v>
       </c>
       <c r="AB17" s="26" t="s">
-        <v>302</v>
-      </c>
-      <c r="AC17" s="10"/>
-      <c r="AD17" s="3">
+        <v>301</v>
+      </c>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="7"/>
+      <c r="AE17" s="29"/>
+      <c r="AF17" s="7"/>
+      <c r="AG17" s="3">
         <v>16</v>
       </c>
-      <c r="AE17" s="20" t="s">
+      <c r="AH17" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="AF17" s="2"/>
+      <c r="AI17" s="2"/>
     </row>
-    <row r="18" spans="1:32" ht="120" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:35" ht="132" customHeight="1">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="1" t="s">
@@ -9110,18 +9629,21 @@
         <v>85</v>
       </c>
       <c r="AB18" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="AC18" s="10"/>
-      <c r="AD18" s="3">
+        <v>300</v>
+      </c>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="7"/>
+      <c r="AE18" s="28"/>
+      <c r="AF18" s="7"/>
+      <c r="AG18" s="3">
         <v>17</v>
       </c>
-      <c r="AE18" s="20" t="s">
+      <c r="AH18" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="AF18" s="2"/>
+      <c r="AI18" s="2"/>
     </row>
-    <row r="19" spans="1:32" ht="120" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:35" ht="135" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="1" t="s">
@@ -9172,18 +9694,21 @@
         <v>86</v>
       </c>
       <c r="AB19" s="20" t="s">
-        <v>310</v>
-      </c>
-      <c r="AC19" s="10"/>
-      <c r="AD19" s="3">
+        <v>309</v>
+      </c>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="7"/>
+      <c r="AE19" s="28"/>
+      <c r="AF19" s="7"/>
+      <c r="AG19" s="3">
         <v>18</v>
       </c>
-      <c r="AE19" s="20" t="s">
+      <c r="AH19" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="AF19" s="2"/>
+      <c r="AI19" s="2"/>
     </row>
-    <row r="20" spans="1:32" ht="140" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:35" ht="149" customHeight="1">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="1" t="s">
@@ -9233,15 +9758,18 @@
         <v>108</v>
       </c>
       <c r="AC20" s="2"/>
-      <c r="AD20" s="3">
+      <c r="AD20" s="7"/>
+      <c r="AE20" s="30"/>
+      <c r="AF20" s="7"/>
+      <c r="AG20" s="3">
         <v>19</v>
       </c>
-      <c r="AE20" s="20" t="s">
+      <c r="AH20" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="AF20" s="2"/>
+      <c r="AI20" s="2"/>
     </row>
-    <row r="21" spans="1:32" ht="140" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:35" ht="147" customHeight="1">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="1" t="s">
@@ -9288,18 +9816,18 @@
         <v>9</v>
       </c>
       <c r="AB21" s="26" t="s">
-        <v>311</v>
-      </c>
-      <c r="AC21" s="10"/>
-      <c r="AD21" s="3">
+        <v>310</v>
+      </c>
+      <c r="AC21" s="2"/>
+      <c r="AG21" s="3">
         <v>20</v>
       </c>
-      <c r="AE21" s="20" t="s">
-        <v>315</v>
-      </c>
-      <c r="AF21" s="2"/>
+      <c r="AH21" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="AI21" s="2"/>
     </row>
-    <row r="22" spans="1:32" ht="120" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:35" ht="136" customHeight="1">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="1" t="s">
@@ -9342,11 +9870,11 @@
         <v>10</v>
       </c>
       <c r="AB22" s="26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AC22" s="2"/>
     </row>
-    <row r="23" spans="1:32" ht="120" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35" ht="144" customHeight="1">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="1" t="s">
@@ -9389,11 +9917,11 @@
         <v>11</v>
       </c>
       <c r="AB23" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AC23" s="2"/>
     </row>
-    <row r="24" spans="1:32" ht="120" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:35" ht="132" customHeight="1">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="1" t="s">
@@ -9436,11 +9964,11 @@
         <v>12</v>
       </c>
       <c r="AB24" s="26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AC24" s="2"/>
     </row>
-    <row r="25" spans="1:32" ht="120" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:35" ht="136" customHeight="1">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="1" t="s">
@@ -9482,7 +10010,7 @@
       <c r="AA25" s="7"/>
       <c r="AC25" s="7"/>
     </row>
-    <row r="26" spans="1:32" ht="120" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:35" ht="136" customHeight="1">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="1" t="s">
@@ -9525,7 +10053,7 @@
       <c r="AB26" s="7"/>
       <c r="AC26" s="7"/>
     </row>
-    <row r="27" spans="1:32" ht="120" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:35" ht="140" customHeight="1">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="1" t="s">
@@ -9565,7 +10093,7 @@
       <c r="Y27" s="12"/>
       <c r="Z27" s="12"/>
     </row>
-    <row r="28" spans="1:32" ht="120" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:35" ht="120">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="1" t="s">
@@ -9608,7 +10136,7 @@
       <c r="AB28" s="7"/>
       <c r="AC28" s="7"/>
     </row>
-    <row r="29" spans="1:32" ht="120" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:35" ht="132" customHeight="1">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="1" t="s">
@@ -9651,7 +10179,7 @@
       <c r="AB29" s="7"/>
       <c r="AC29" s="7"/>
     </row>
-    <row r="30" spans="1:32" ht="120" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:35" ht="132" customHeight="1">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="1" t="s">
@@ -9694,7 +10222,7 @@
       <c r="AB30" s="7"/>
       <c r="AC30" s="7"/>
     </row>
-    <row r="31" spans="1:32" ht="120" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:35" ht="140" customHeight="1">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="1" t="s">
@@ -9737,7 +10265,7 @@
       <c r="AB31" s="7"/>
       <c r="AC31" s="7"/>
     </row>
-    <row r="32" spans="1:32" ht="120" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:35" ht="136" customHeight="1">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="1" t="s">
@@ -9780,7 +10308,7 @@
       <c r="AB32" s="7"/>
       <c r="AC32" s="7"/>
     </row>
-    <row r="33" spans="1:29" ht="120" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" ht="132" customHeight="1">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="1" t="s">
@@ -9823,7 +10351,7 @@
       <c r="AB33" s="7"/>
       <c r="AC33" s="7"/>
     </row>
-    <row r="34" spans="1:29" ht="120" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" ht="120">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="1" t="s">
@@ -9862,7 +10390,7 @@
       <c r="AB34" s="7"/>
       <c r="AC34" s="7"/>
     </row>
-    <row r="35" spans="1:29" ht="120" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:29" ht="144" customHeight="1">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="1" t="s">
@@ -9898,7 +10426,7 @@
       <c r="AB35" s="7"/>
       <c r="AC35" s="7"/>
     </row>
-    <row r="36" spans="1:29" ht="120" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:29" ht="140" customHeight="1">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="1" t="s">
@@ -9924,7 +10452,7 @@
       <c r="Y36" s="7"/>
       <c r="Z36" s="7"/>
     </row>
-    <row r="37" spans="1:29" ht="120" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" ht="132" customHeight="1">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="1" t="s">
@@ -9951,8 +10479,8 @@
       <c r="Z37" s="7"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="OWCc3zesiE16HqNRi/A5iDC7XvguOX/SP+U+xNNLorfW7CI6CrclNlJaVQIwIg2Lk4uJkkzy68OXc7K7bNKWAw==" saltValue="6L+xI85r6LUJM9Tx1uM5tQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <dataValidations count="20">
+  <sheetProtection algorithmName="SHA-512" hashValue="s0kj3JKUqpS8Pu5oOmKoekjSTEoRtb2FClQmP8okltXs0cLq9iyGH0JXzfZ4ajeWBVrjUKJ0bMNGBWCllBwslg==" saltValue="SechR6wV6VU5TbQsdjmE1A==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <dataValidations count="19">
     <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Name must be less than 20 characters_x000a_" sqref="B5 B2" xr:uid="{91D9CADE-1361-894F-81E5-FC375AB75B27}">
       <formula1>19</formula1>
     </dataValidation>
@@ -9996,18 +10524,18 @@
       <formula1>0</formula1>
       <formula2>3</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input a number between 0 and 4" sqref="AC21:AC24 AC2:AC9 W2:W21 AF2:AF21" xr:uid="{F7AEEDA1-C641-A946-B2D6-50CF8F25AB41}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input a number between 0 and 4" sqref="AC21:AC24 AC2:AC9 W2:W21 AF2:AF16 AI2:AI21" xr:uid="{F7AEEDA1-C641-A946-B2D6-50CF8F25AB41}">
       <formula1>0</formula1>
       <formula2>4</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input either 'Y' or 'N'" sqref="AC10:AC19" xr:uid="{C45CB5A2-312A-9349-BC4A-AA78049DC6D5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input either 'Y' or 'N'" sqref="AC10:AC19 AF17:AF19" xr:uid="{C45CB5A2-312A-9349-BC4A-AA78049DC6D5}">
       <formula1>"Y, N"</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Input a number between 1 and 5." sqref="H2:H35" xr:uid="{C5C022E8-27A2-0343-A204-FA487880999E}">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Message must be less than 40 characters" sqref="AC20" xr:uid="{D33F11B3-65C5-1F4F-93EC-CA5ED38EB5A9}">
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Message must be less than 40 characters" sqref="AC20 AF20" xr:uid="{D33F11B3-65C5-1F4F-93EC-CA5ED38EB5A9}">
       <formula1>40</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Enter either 'Y' or 'N'" sqref="K2:K11 K13:K16 K30:K32 K18:K28" xr:uid="{B18B96E8-2046-B24C-850F-5D4B23987964}">
@@ -10016,10 +10544,7 @@
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" sqref="K12 K17 K29 K33" xr:uid="{7CC4C9CF-B45E-3D4B-9044-97043DD3C98F}">
       <formula1>40</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Enter DOB in format DD/MM/YY" sqref="B7" xr:uid="{B971CFD9-E350-D645-8852-63D322A3CEE8}">
-      <formula1>47848</formula1>
-    </dataValidation>
-    <dataValidation type="date" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Enter DOB in format DD/MM/YY" sqref="B6" xr:uid="{7007CAA5-60C3-C44F-9AED-62FF3561C751}">
+    <dataValidation type="date" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Enter DOB in format DD/MM/YY" sqref="B6:B7" xr:uid="{B971CFD9-E350-D645-8852-63D322A3CEE8}">
       <formula1>47848</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>